<commit_message>
Working grade lvl and floor restriction
</commit_message>
<xml_diff>
--- a/lib/CVHS Locker Template and Guide.xlsx
+++ b/lib/CVHS Locker Template and Guide.xlsx
@@ -44588,7 +44588,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B96"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -44804,561 +44804,553 @@
     </row>
     <row r="27" spans="1:2" customFormat="false">
       <c r="A27" t="s">
-        <v>2093</v>
+        <v>2095</v>
       </c>
       <c r="B27" t="s">
-        <v>2094</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="28" spans="1:2" customFormat="false">
       <c r="A28" t="s">
-        <v>2095</v>
+        <v>2097</v>
       </c>
       <c r="B28" t="s">
-        <v>2096</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="29" spans="1:2" customFormat="false">
       <c r="A29" t="s">
-        <v>2097</v>
+        <v>2099</v>
       </c>
       <c r="B29" t="s">
-        <v>2098</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="30" spans="1:2" customFormat="false">
       <c r="A30" t="s">
-        <v>2099</v>
+        <v>2101</v>
       </c>
       <c r="B30" t="s">
-        <v>2100</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="31" spans="1:2" customFormat="false">
       <c r="A31" t="s">
-        <v>2101</v>
+        <v>2103</v>
       </c>
       <c r="B31" t="s">
-        <v>2102</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="32" spans="1:2" customFormat="false">
       <c r="A32" t="s">
-        <v>2103</v>
+        <v>2105</v>
       </c>
       <c r="B32" t="s">
-        <v>2104</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="33" spans="1:2" customFormat="false">
       <c r="A33" t="s">
-        <v>2105</v>
+        <v>2107</v>
       </c>
       <c r="B33" t="s">
-        <v>2106</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="34" spans="1:2" customFormat="false">
       <c r="A34" t="s">
-        <v>2107</v>
+        <v>2109</v>
       </c>
       <c r="B34" t="s">
-        <v>2108</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="35" spans="1:2" customFormat="false">
       <c r="A35" t="s">
-        <v>2109</v>
+        <v>2111</v>
       </c>
       <c r="B35" t="s">
-        <v>2110</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="36" spans="1:2" customFormat="false">
       <c r="A36" t="s">
-        <v>2111</v>
+        <v>2113</v>
       </c>
       <c r="B36" t="s">
-        <v>2112</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="37" spans="1:2" customFormat="false">
       <c r="A37" t="s">
-        <v>2113</v>
+        <v>2115</v>
       </c>
       <c r="B37" t="s">
-        <v>2114</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="38" spans="1:2" customFormat="false">
       <c r="A38" t="s">
-        <v>2115</v>
+        <v>2117</v>
       </c>
       <c r="B38" t="s">
-        <v>2116</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="39" spans="1:2" customFormat="false">
       <c r="A39" t="s">
-        <v>2117</v>
+        <v>2119</v>
       </c>
       <c r="B39" t="s">
-        <v>2118</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="40" spans="1:2" customFormat="false">
       <c r="A40" t="s">
-        <v>2119</v>
+        <v>2121</v>
       </c>
       <c r="B40" t="s">
-        <v>2120</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="41" spans="1:2" customFormat="false">
       <c r="A41" t="s">
-        <v>2121</v>
+        <v>2123</v>
       </c>
       <c r="B41" t="s">
-        <v>2122</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="42" spans="1:2" customFormat="false">
       <c r="A42" t="s">
-        <v>2123</v>
+        <v>2125</v>
       </c>
       <c r="B42" t="s">
-        <v>2124</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="43" spans="1:2" customFormat="false">
       <c r="A43" t="s">
-        <v>2125</v>
+        <v>2127</v>
       </c>
       <c r="B43" t="s">
-        <v>2126</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="44" spans="1:2" customFormat="false">
       <c r="A44" t="s">
-        <v>2127</v>
+        <v>2129</v>
       </c>
       <c r="B44" t="s">
-        <v>2128</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="45" spans="1:2" customFormat="false">
       <c r="A45" t="s">
-        <v>2129</v>
+        <v>2131</v>
       </c>
       <c r="B45" t="s">
-        <v>2130</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="46" spans="1:2" customFormat="false">
       <c r="A46" t="s">
-        <v>2131</v>
+        <v>2133</v>
       </c>
       <c r="B46" t="s">
-        <v>2132</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="47" spans="1:2" customFormat="false">
       <c r="A47" t="s">
-        <v>2133</v>
+        <v>2135</v>
       </c>
       <c r="B47" t="s">
-        <v>2134</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="48" spans="1:2" customFormat="false">
       <c r="A48" t="s">
-        <v>2135</v>
+        <v>2137</v>
       </c>
       <c r="B48" t="s">
-        <v>2136</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="49" spans="1:2" customFormat="false">
       <c r="A49" t="s">
-        <v>2137</v>
+        <v>2139</v>
       </c>
       <c r="B49" t="s">
-        <v>2138</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="50" spans="1:2" customFormat="false">
       <c r="A50" t="s">
-        <v>2139</v>
+        <v>2143</v>
       </c>
       <c r="B50" t="s">
-        <v>2140</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="51" spans="1:2" customFormat="false">
       <c r="A51" t="s">
-        <v>2143</v>
+        <v>2145</v>
       </c>
       <c r="B51" t="s">
-        <v>2144</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="52" spans="1:2" customFormat="false">
       <c r="A52" t="s">
-        <v>2145</v>
+        <v>2147</v>
       </c>
       <c r="B52" t="s">
-        <v>2146</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="53" spans="1:2" customFormat="false">
       <c r="A53" t="s">
-        <v>2147</v>
+        <v>2149</v>
       </c>
       <c r="B53" t="s">
-        <v>2148</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="54" spans="1:2" customFormat="false">
       <c r="A54" t="s">
-        <v>2149</v>
+        <v>2151</v>
       </c>
       <c r="B54" t="s">
-        <v>2150</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="55" spans="1:2" customFormat="false">
       <c r="A55" t="s">
-        <v>2151</v>
+        <v>2153</v>
       </c>
       <c r="B55" t="s">
-        <v>2152</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="56" spans="1:2" customFormat="false">
       <c r="A56" t="s">
-        <v>2153</v>
+        <v>2155</v>
       </c>
       <c r="B56" t="s">
-        <v>2154</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="57" spans="1:2" customFormat="false">
       <c r="A57" t="s">
-        <v>2155</v>
+        <v>2157</v>
       </c>
       <c r="B57" t="s">
-        <v>2156</v>
+        <v>2158</v>
       </c>
     </row>
     <row r="58" spans="1:2" customFormat="false">
       <c r="A58" t="s">
-        <v>2157</v>
+        <v>2159</v>
       </c>
       <c r="B58" t="s">
-        <v>2158</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="59" spans="1:2" customFormat="false">
       <c r="A59" t="s">
-        <v>2159</v>
+        <v>2161</v>
       </c>
       <c r="B59" t="s">
-        <v>2160</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="60" spans="1:2" customFormat="false">
       <c r="A60" t="s">
-        <v>2161</v>
+        <v>2163</v>
       </c>
       <c r="B60" t="s">
-        <v>2162</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="61" spans="1:2" customFormat="false">
       <c r="A61" t="s">
-        <v>2163</v>
+        <v>2165</v>
       </c>
       <c r="B61" t="s">
-        <v>2164</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="62" spans="1:2" customFormat="false">
       <c r="A62" t="s">
-        <v>2165</v>
+        <v>2167</v>
       </c>
       <c r="B62" t="s">
-        <v>2166</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="63" spans="1:2" customFormat="false">
       <c r="A63" t="s">
-        <v>2167</v>
+        <v>2169</v>
       </c>
       <c r="B63" t="s">
-        <v>2168</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="64" spans="1:2" customFormat="false">
       <c r="A64" t="s">
-        <v>2169</v>
+        <v>2171</v>
       </c>
       <c r="B64" t="s">
-        <v>2170</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="65" spans="1:2" customFormat="false">
       <c r="A65" t="s">
-        <v>2171</v>
+        <v>2173</v>
       </c>
       <c r="B65" t="s">
-        <v>2172</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="66" spans="1:2" customFormat="false">
       <c r="A66" t="s">
-        <v>2173</v>
+        <v>2175</v>
       </c>
       <c r="B66" t="s">
-        <v>2174</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="67" spans="1:2" customFormat="false">
       <c r="A67" t="s">
-        <v>2175</v>
+        <v>2177</v>
       </c>
       <c r="B67" t="s">
-        <v>2176</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="68" spans="1:2" customFormat="false">
       <c r="A68" t="s">
-        <v>2177</v>
+        <v>2179</v>
       </c>
       <c r="B68" t="s">
-        <v>2178</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="69" spans="1:2" customFormat="false">
       <c r="A69" t="s">
-        <v>2179</v>
+        <v>2181</v>
       </c>
       <c r="B69" t="s">
-        <v>2180</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="70" spans="1:2" customFormat="false">
       <c r="A70" t="s">
-        <v>2181</v>
+        <v>2183</v>
       </c>
       <c r="B70" t="s">
-        <v>2182</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="71" spans="1:2" customFormat="false">
       <c r="A71" t="s">
-        <v>2183</v>
+        <v>2185</v>
       </c>
       <c r="B71" t="s">
-        <v>2184</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="72" spans="1:2" customFormat="false">
       <c r="A72" t="s">
-        <v>2185</v>
+        <v>2187</v>
       </c>
       <c r="B72" t="s">
-        <v>2186</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="73" spans="1:2" customFormat="false">
       <c r="A73" t="s">
-        <v>2187</v>
+        <v>2189</v>
       </c>
       <c r="B73" t="s">
-        <v>2188</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="74" spans="1:2" customFormat="false">
       <c r="A74" t="s">
-        <v>2189</v>
+        <v>2191</v>
       </c>
       <c r="B74" t="s">
-        <v>2190</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="75" spans="1:2" customFormat="false">
       <c r="A75" t="s">
-        <v>2191</v>
+        <v>2193</v>
       </c>
       <c r="B75" t="s">
-        <v>2192</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="76" spans="1:2" customFormat="false">
       <c r="A76" t="s">
-        <v>2193</v>
+        <v>2195</v>
       </c>
       <c r="B76" t="s">
-        <v>2194</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="77" spans="1:2" customFormat="false">
       <c r="A77" t="s">
-        <v>2195</v>
+        <v>2199</v>
       </c>
       <c r="B77" t="s">
-        <v>2196</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="78" spans="1:2" customFormat="false">
       <c r="A78" t="s">
-        <v>2199</v>
+        <v>2201</v>
       </c>
       <c r="B78" t="s">
-        <v>2200</v>
+        <v>2202</v>
       </c>
     </row>
     <row r="79" spans="1:2" customFormat="false">
       <c r="A79" t="s">
-        <v>2201</v>
+        <v>2203</v>
       </c>
       <c r="B79" t="s">
-        <v>2202</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="80" spans="1:2" customFormat="false">
       <c r="A80" t="s">
-        <v>2203</v>
+        <v>2205</v>
       </c>
       <c r="B80" t="s">
-        <v>2204</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="81" spans="1:2" customFormat="false">
       <c r="A81" t="s">
-        <v>2205</v>
+        <v>2207</v>
       </c>
       <c r="B81" t="s">
-        <v>2206</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="82" spans="1:2" customFormat="false">
       <c r="A82" t="s">
-        <v>2207</v>
+        <v>2209</v>
       </c>
       <c r="B82" t="s">
-        <v>2208</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="83" spans="1:2" customFormat="false">
       <c r="A83" t="s">
-        <v>2209</v>
+        <v>2211</v>
       </c>
       <c r="B83" t="s">
-        <v>2210</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="84" spans="1:2" customFormat="false">
       <c r="A84" t="s">
-        <v>2211</v>
+        <v>2213</v>
       </c>
       <c r="B84" t="s">
-        <v>2212</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="85" spans="1:2" customFormat="false">
       <c r="A85" t="s">
-        <v>2213</v>
+        <v>2215</v>
       </c>
       <c r="B85" t="s">
-        <v>2214</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="86" spans="1:2" customFormat="false">
       <c r="A86" t="s">
-        <v>2215</v>
+        <v>2217</v>
       </c>
       <c r="B86" t="s">
-        <v>2216</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="87" spans="1:2" customFormat="false">
       <c r="A87" t="s">
-        <v>2217</v>
+        <v>2219</v>
       </c>
       <c r="B87" t="s">
-        <v>2218</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="88" spans="1:2" customFormat="false">
       <c r="A88" t="s">
-        <v>2219</v>
+        <v>2221</v>
       </c>
       <c r="B88" t="s">
-        <v>2220</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="89" spans="1:2" customFormat="false">
       <c r="A89" t="s">
-        <v>2221</v>
+        <v>2223</v>
       </c>
       <c r="B89" t="s">
-        <v>2222</v>
+        <v>2224</v>
       </c>
     </row>
     <row r="90" spans="1:2" customFormat="false">
       <c r="A90" t="s">
-        <v>2223</v>
+        <v>2225</v>
       </c>
       <c r="B90" t="s">
-        <v>2224</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="91" spans="1:2" customFormat="false">
       <c r="A91" t="s">
-        <v>2225</v>
+        <v>2227</v>
       </c>
       <c r="B91" t="s">
-        <v>2226</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="92" spans="1:2" customFormat="false">
       <c r="A92" t="s">
-        <v>2227</v>
+        <v>2229</v>
       </c>
       <c r="B92" t="s">
-        <v>2228</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="93" spans="1:2" customFormat="false">
       <c r="A93" t="s">
-        <v>2229</v>
+        <v>2231</v>
       </c>
       <c r="B93" t="s">
-        <v>2230</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="94" spans="1:2" customFormat="false">
-      <c r="A94" t="s">
-        <v>2231</v>
-      </c>
-      <c r="B94" t="s">
-        <v>2232</v>
+      <c r="A94" s="0" t="str">
+        <v>72079</v>
+      </c>
+      <c r="B94" s="0" t="str">
+        <v>1005693</v>
       </c>
     </row>
     <row r="95" spans="1:2" customFormat="false">
       <c r="A95" s="0" t="str">
-        <v>72079</v>
+        <v>72051</v>
       </c>
       <c r="B95" s="0" t="str">
-        <v>1005693</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" customFormat="false">
-      <c r="A96" s="0" t="str">
-        <v>72051</v>
-      </c>
-      <c r="B96" s="0" t="str">
         <v>1005665</v>
       </c>
     </row>
@@ -46134,7 +46126,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
@@ -46188,6 +46180,22 @@
       </c>
       <c r="B6" s="0" t="str">
         <v>1005174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" customFormat="false">
+      <c r="A7" s="0" t="str">
+        <v>406527</v>
+      </c>
+      <c r="B7" s="0" t="str">
+        <v>1005641</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" customFormat="false">
+      <c r="A8" s="0" t="str">
+        <v>412462</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <v>1005641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed get gradelvl bug and error with letters
</commit_message>
<xml_diff>
--- a/lib/CVHS Locker Template and Guide.xlsx
+++ b/lib/CVHS Locker Template and Guide.xlsx
@@ -36042,42 +36042,42 @@
     </row>
     <row r="164" spans="1:2" customFormat="false">
       <c r="A164" s="0" t="str">
-        <v>53183</v>
+        <v>53185</v>
       </c>
       <c r="B164" s="0" t="str">
-        <v>1005454</v>
+        <v>1005455</v>
       </c>
     </row>
     <row r="165" spans="1:2" customFormat="false">
       <c r="A165" s="0" t="str">
-        <v>53185</v>
+        <v>53187</v>
       </c>
       <c r="B165" s="0" t="str">
-        <v>1005455</v>
+        <v>1005456</v>
       </c>
     </row>
     <row r="166" spans="1:2" customFormat="false">
       <c r="A166" s="0" t="str">
-        <v>53187</v>
+        <v>53189</v>
       </c>
       <c r="B166" s="0" t="str">
-        <v>1005456</v>
+        <v>1005457</v>
       </c>
     </row>
     <row r="167" spans="1:2" customFormat="false">
       <c r="A167" s="0" t="str">
-        <v>53189</v>
+        <v>53191</v>
       </c>
       <c r="B167" s="0" t="str">
-        <v>1005457</v>
+        <v>1005458</v>
       </c>
     </row>
     <row r="168" spans="1:2" customFormat="false">
       <c r="A168" s="0" t="str">
-        <v>53191</v>
+        <v>53183</v>
       </c>
       <c r="B168" s="0" t="str">
-        <v>1005458</v>
+        <v>1005454</v>
       </c>
     </row>
   </sheetData>
@@ -37154,186 +37154,186 @@
     </row>
     <row r="134" spans="1:2" customFormat="false">
       <c r="A134" s="0" t="str">
-        <v>71134</v>
+        <v>71135</v>
       </c>
       <c r="B134" s="0" t="str">
-        <v>1005592</v>
+        <v>1005593</v>
       </c>
     </row>
     <row r="135" spans="1:2" customFormat="false">
       <c r="A135" s="0" t="str">
-        <v>71135</v>
+        <v>71136</v>
       </c>
       <c r="B135" s="0" t="str">
-        <v>1005593</v>
+        <v>1005594</v>
       </c>
     </row>
     <row r="136" spans="1:2" customFormat="false">
       <c r="A136" s="0" t="str">
-        <v>71136</v>
+        <v>71137</v>
       </c>
       <c r="B136" s="0" t="str">
-        <v>1005594</v>
+        <v>1005595</v>
       </c>
     </row>
     <row r="137" spans="1:2" customFormat="false">
       <c r="A137" s="0" t="str">
-        <v>71137</v>
+        <v>71138</v>
       </c>
       <c r="B137" s="0" t="str">
-        <v>1005595</v>
+        <v>1005596</v>
       </c>
     </row>
     <row r="138" spans="1:2" customFormat="false">
       <c r="A138" s="0" t="str">
-        <v>71138</v>
+        <v>71139</v>
       </c>
       <c r="B138" s="0" t="str">
-        <v>1005596</v>
+        <v>1005597</v>
       </c>
     </row>
     <row r="139" spans="1:2" customFormat="false">
       <c r="A139" s="0" t="str">
-        <v>71139</v>
+        <v>71140</v>
       </c>
       <c r="B139" s="0" t="str">
-        <v>1005597</v>
+        <v>1005598</v>
       </c>
     </row>
     <row r="140" spans="1:2" customFormat="false">
       <c r="A140" s="0" t="str">
-        <v>71140</v>
+        <v>71141</v>
       </c>
       <c r="B140" s="0" t="str">
-        <v>1005598</v>
+        <v>1005599</v>
       </c>
     </row>
     <row r="141" spans="1:2" customFormat="false">
       <c r="A141" s="0" t="str">
-        <v>71141</v>
+        <v>71142</v>
       </c>
       <c r="B141" s="0" t="str">
-        <v>1005599</v>
+        <v>1005600</v>
       </c>
     </row>
     <row r="142" spans="1:2" customFormat="false">
       <c r="A142" s="0" t="str">
-        <v>71142</v>
+        <v>71143</v>
       </c>
       <c r="B142" s="0" t="str">
-        <v>1005600</v>
+        <v>1005601</v>
       </c>
     </row>
     <row r="143" spans="1:2" customFormat="false">
       <c r="A143" s="0" t="str">
-        <v>71143</v>
+        <v>71144</v>
       </c>
       <c r="B143" s="0" t="str">
-        <v>1005601</v>
+        <v>1005602</v>
       </c>
     </row>
     <row r="144" spans="1:2" customFormat="false">
       <c r="A144" s="0" t="str">
-        <v>71144</v>
+        <v>71145</v>
       </c>
       <c r="B144" s="0" t="str">
-        <v>1005602</v>
+        <v>1005603</v>
       </c>
     </row>
     <row r="145" spans="1:2" customFormat="false">
       <c r="A145" s="0" t="str">
-        <v>71145</v>
+        <v>71146</v>
       </c>
       <c r="B145" s="0" t="str">
-        <v>1005603</v>
+        <v>1005604</v>
       </c>
     </row>
     <row r="146" spans="1:2" customFormat="false">
       <c r="A146" s="0" t="str">
-        <v>71146</v>
+        <v>71147</v>
       </c>
       <c r="B146" s="0" t="str">
-        <v>1005604</v>
+        <v>1005605</v>
       </c>
     </row>
     <row r="147" spans="1:2" customFormat="false">
       <c r="A147" s="0" t="str">
-        <v>71147</v>
+        <v>71148</v>
       </c>
       <c r="B147" s="0" t="str">
-        <v>1005605</v>
+        <v>1005606</v>
       </c>
     </row>
     <row r="148" spans="1:2" customFormat="false">
       <c r="A148" s="0" t="str">
-        <v>71148</v>
+        <v>71149</v>
       </c>
       <c r="B148" s="0" t="str">
-        <v>1005606</v>
+        <v>1005607</v>
       </c>
     </row>
     <row r="149" spans="1:2" customFormat="false">
       <c r="A149" s="0" t="str">
-        <v>71149</v>
+        <v>71150</v>
       </c>
       <c r="B149" s="0" t="str">
-        <v>1005607</v>
+        <v>1005608</v>
       </c>
     </row>
     <row r="150" spans="1:2" customFormat="false">
       <c r="A150" s="0" t="str">
-        <v>71150</v>
+        <v>71151</v>
       </c>
       <c r="B150" s="0" t="str">
-        <v>1005608</v>
+        <v>1005609</v>
       </c>
     </row>
     <row r="151" spans="1:2" customFormat="false">
       <c r="A151" s="0" t="str">
-        <v>71151</v>
+        <v>71152</v>
       </c>
       <c r="B151" s="0" t="str">
-        <v>1005609</v>
+        <v>1005610</v>
       </c>
     </row>
     <row r="152" spans="1:2" customFormat="false">
       <c r="A152" s="0" t="str">
-        <v>71152</v>
+        <v>71153</v>
       </c>
       <c r="B152" s="0" t="str">
-        <v>1005610</v>
+        <v>1005611</v>
       </c>
     </row>
     <row r="153" spans="1:2" customFormat="false">
       <c r="A153" s="0" t="str">
-        <v>71153</v>
+        <v>71155</v>
       </c>
       <c r="B153" s="0" t="str">
-        <v>1005611</v>
+        <v>1005612</v>
       </c>
     </row>
     <row r="154" spans="1:2" customFormat="false">
       <c r="A154" s="0" t="str">
-        <v>71155</v>
+        <v>71157</v>
       </c>
       <c r="B154" s="0" t="str">
-        <v>1005612</v>
+        <v>1005613</v>
       </c>
     </row>
     <row r="155" spans="1:2" customFormat="false">
       <c r="A155" s="0" t="str">
-        <v>71157</v>
+        <v>71159</v>
       </c>
       <c r="B155" s="0" t="str">
-        <v>1005613</v>
+        <v>1005614</v>
       </c>
     </row>
     <row r="156" spans="1:2" customFormat="false">
       <c r="A156" s="0" t="str">
-        <v>71159</v>
+        <v>71134</v>
       </c>
       <c r="B156" s="0" t="str">
-        <v>1005614</v>
+        <v>1005592</v>
       </c>
     </row>
   </sheetData>
@@ -50666,322 +50666,322 @@
     </row>
     <row r="57" spans="1:2" customFormat="false">
       <c r="A57" s="0" t="str">
-        <v>52057</v>
+        <v>52058</v>
       </c>
       <c r="B57" s="0" t="str">
-        <v>1005251</v>
+        <v>1005252</v>
       </c>
     </row>
     <row r="58" spans="1:2" customFormat="false">
       <c r="A58" s="0" t="str">
-        <v>52058</v>
+        <v>52059</v>
       </c>
       <c r="B58" s="0" t="str">
-        <v>1005252</v>
+        <v>1005253</v>
       </c>
     </row>
     <row r="59" spans="1:2" customFormat="false">
       <c r="A59" s="0" t="str">
-        <v>52059</v>
+        <v>52060</v>
       </c>
       <c r="B59" s="0" t="str">
-        <v>1005253</v>
+        <v>1005254</v>
       </c>
     </row>
     <row r="60" spans="1:2" customFormat="false">
       <c r="A60" s="0" t="str">
-        <v>52060</v>
+        <v>52061</v>
       </c>
       <c r="B60" s="0" t="str">
-        <v>1005254</v>
+        <v>1005255</v>
       </c>
     </row>
     <row r="61" spans="1:2" customFormat="false">
       <c r="A61" s="0" t="str">
-        <v>52061</v>
+        <v>52062</v>
       </c>
       <c r="B61" s="0" t="str">
-        <v>1005255</v>
+        <v>1005256</v>
       </c>
     </row>
     <row r="62" spans="1:2" customFormat="false">
       <c r="A62" s="0" t="str">
-        <v>52062</v>
+        <v>52063</v>
       </c>
       <c r="B62" s="0" t="str">
-        <v>1005256</v>
+        <v>1005257</v>
       </c>
     </row>
     <row r="63" spans="1:2" customFormat="false">
       <c r="A63" s="0" t="str">
-        <v>52063</v>
+        <v>52064</v>
       </c>
       <c r="B63" s="0" t="str">
-        <v>1005257</v>
+        <v>1005258</v>
       </c>
     </row>
     <row r="64" spans="1:2" customFormat="false">
       <c r="A64" s="0" t="str">
-        <v>52064</v>
+        <v>52065</v>
       </c>
       <c r="B64" s="0" t="str">
-        <v>1005258</v>
+        <v>1005259</v>
       </c>
     </row>
     <row r="65" spans="1:2" customFormat="false">
       <c r="A65" s="0" t="str">
-        <v>52065</v>
+        <v>52066</v>
       </c>
       <c r="B65" s="0" t="str">
-        <v>1005259</v>
+        <v>1005260</v>
       </c>
     </row>
     <row r="66" spans="1:2" customFormat="false">
       <c r="A66" s="0" t="str">
-        <v>52066</v>
+        <v>52067</v>
       </c>
       <c r="B66" s="0" t="str">
-        <v>1005260</v>
+        <v>1005261</v>
       </c>
     </row>
     <row r="67" spans="1:2" customFormat="false">
       <c r="A67" s="0" t="str">
-        <v>52067</v>
+        <v>52068</v>
       </c>
       <c r="B67" s="0" t="str">
-        <v>1005261</v>
+        <v>1005262</v>
       </c>
     </row>
     <row r="68" spans="1:2" customFormat="false">
       <c r="A68" s="0" t="str">
-        <v>52068</v>
+        <v>52069</v>
       </c>
       <c r="B68" s="0" t="str">
-        <v>1005262</v>
+        <v>1005263</v>
       </c>
     </row>
     <row r="69" spans="1:2" customFormat="false">
       <c r="A69" s="0" t="str">
-        <v>52069</v>
+        <v>52070</v>
       </c>
       <c r="B69" s="0" t="str">
-        <v>1005263</v>
+        <v>1005264</v>
       </c>
     </row>
     <row r="70" spans="1:2" customFormat="false">
       <c r="A70" s="0" t="str">
-        <v>52070</v>
+        <v>52071</v>
       </c>
       <c r="B70" s="0" t="str">
-        <v>1005264</v>
+        <v>1005265</v>
       </c>
     </row>
     <row r="71" spans="1:2" customFormat="false">
       <c r="A71" s="0" t="str">
-        <v>52071</v>
+        <v>52072</v>
       </c>
       <c r="B71" s="0" t="str">
-        <v>1005265</v>
+        <v>1005266</v>
       </c>
     </row>
     <row r="72" spans="1:2" customFormat="false">
       <c r="A72" s="0" t="str">
-        <v>52072</v>
+        <v>52073</v>
       </c>
       <c r="B72" s="0" t="str">
-        <v>1005266</v>
+        <v>1005267</v>
       </c>
     </row>
     <row r="73" spans="1:2" customFormat="false">
       <c r="A73" s="0" t="str">
-        <v>52073</v>
+        <v>52074</v>
       </c>
       <c r="B73" s="0" t="str">
-        <v>1005267</v>
+        <v>1005268</v>
       </c>
     </row>
     <row r="74" spans="1:2" customFormat="false">
       <c r="A74" s="0" t="str">
-        <v>52074</v>
+        <v>52075</v>
       </c>
       <c r="B74" s="0" t="str">
-        <v>1005268</v>
+        <v>1005269</v>
       </c>
     </row>
     <row r="75" spans="1:2" customFormat="false">
       <c r="A75" s="0" t="str">
-        <v>52075</v>
+        <v>52076</v>
       </c>
       <c r="B75" s="0" t="str">
-        <v>1005269</v>
+        <v>1005270</v>
       </c>
     </row>
     <row r="76" spans="1:2" customFormat="false">
       <c r="A76" s="0" t="str">
-        <v>52076</v>
+        <v>52077</v>
       </c>
       <c r="B76" s="0" t="str">
-        <v>1005270</v>
+        <v>1005271</v>
       </c>
     </row>
     <row r="77" spans="1:2" customFormat="false">
       <c r="A77" s="0" t="str">
-        <v>52077</v>
+        <v>52078</v>
       </c>
       <c r="B77" s="0" t="str">
-        <v>1005271</v>
+        <v>1005272</v>
       </c>
     </row>
     <row r="78" spans="1:2" customFormat="false">
       <c r="A78" s="0" t="str">
-        <v>52078</v>
+        <v>52079</v>
       </c>
       <c r="B78" s="0" t="str">
-        <v>1005272</v>
+        <v>1005273</v>
       </c>
     </row>
     <row r="79" spans="1:2" customFormat="false">
       <c r="A79" s="0" t="str">
-        <v>52079</v>
+        <v>52080</v>
       </c>
       <c r="B79" s="0" t="str">
-        <v>1005273</v>
+        <v>1005274</v>
       </c>
     </row>
     <row r="80" spans="1:2" customFormat="false">
       <c r="A80" s="0" t="str">
-        <v>52080</v>
+        <v>52081</v>
       </c>
       <c r="B80" s="0" t="str">
-        <v>1005274</v>
+        <v>1005275</v>
       </c>
     </row>
     <row r="81" spans="1:2" customFormat="false">
       <c r="A81" s="0" t="str">
-        <v>52081</v>
+        <v>52082</v>
       </c>
       <c r="B81" s="0" t="str">
-        <v>1005275</v>
+        <v>1005276</v>
       </c>
     </row>
     <row r="82" spans="1:2" customFormat="false">
       <c r="A82" s="0" t="str">
-        <v>52082</v>
+        <v>52083</v>
       </c>
       <c r="B82" s="0" t="str">
-        <v>1005276</v>
+        <v>1005277</v>
       </c>
     </row>
     <row r="83" spans="1:2" customFormat="false">
       <c r="A83" s="0" t="str">
-        <v>52083</v>
+        <v>52084</v>
       </c>
       <c r="B83" s="0" t="str">
-        <v>1005277</v>
+        <v>1005278</v>
       </c>
     </row>
     <row r="84" spans="1:2" customFormat="false">
       <c r="A84" s="0" t="str">
-        <v>52084</v>
+        <v>52085</v>
       </c>
       <c r="B84" s="0" t="str">
-        <v>1005278</v>
+        <v>1005279</v>
       </c>
     </row>
     <row r="85" spans="1:2" customFormat="false">
       <c r="A85" s="0" t="str">
-        <v>52085</v>
+        <v>52086</v>
       </c>
       <c r="B85" s="0" t="str">
-        <v>1005279</v>
+        <v>1005280</v>
       </c>
     </row>
     <row r="86" spans="1:2" customFormat="false">
       <c r="A86" s="0" t="str">
-        <v>52086</v>
+        <v>52087</v>
       </c>
       <c r="B86" s="0" t="str">
-        <v>1005280</v>
+        <v>1005281</v>
       </c>
     </row>
     <row r="87" spans="1:2" customFormat="false">
       <c r="A87" s="0" t="str">
-        <v>52087</v>
+        <v>52088</v>
       </c>
       <c r="B87" s="0" t="str">
-        <v>1005281</v>
+        <v>1005282</v>
       </c>
     </row>
     <row r="88" spans="1:2" customFormat="false">
       <c r="A88" s="0" t="str">
-        <v>52088</v>
+        <v>52089</v>
       </c>
       <c r="B88" s="0" t="str">
-        <v>1005282</v>
+        <v>1005283</v>
       </c>
     </row>
     <row r="89" spans="1:2" customFormat="false">
       <c r="A89" s="0" t="str">
-        <v>52089</v>
+        <v>52090</v>
       </c>
       <c r="B89" s="0" t="str">
-        <v>1005283</v>
+        <v>1005284</v>
       </c>
     </row>
     <row r="90" spans="1:2" customFormat="false">
       <c r="A90" s="0" t="str">
-        <v>52090</v>
+        <v>52091</v>
       </c>
       <c r="B90" s="0" t="str">
-        <v>1005284</v>
+        <v>1005285</v>
       </c>
     </row>
     <row r="91" spans="1:2" customFormat="false">
       <c r="A91" s="0" t="str">
-        <v>52091</v>
+        <v>52092</v>
       </c>
       <c r="B91" s="0" t="str">
-        <v>1005285</v>
+        <v>1005286</v>
       </c>
     </row>
     <row r="92" spans="1:2" customFormat="false">
       <c r="A92" s="0" t="str">
-        <v>52092</v>
+        <v>52093</v>
       </c>
       <c r="B92" s="0" t="str">
-        <v>1005286</v>
+        <v>1005287</v>
       </c>
     </row>
     <row r="93" spans="1:2" customFormat="false">
       <c r="A93" s="0" t="str">
-        <v>52093</v>
+        <v>52094</v>
       </c>
       <c r="B93" s="0" t="str">
-        <v>1005287</v>
+        <v>1005288</v>
       </c>
     </row>
     <row r="94" spans="1:2" customFormat="false">
       <c r="A94" s="0" t="str">
-        <v>52094</v>
+        <v>52095</v>
       </c>
       <c r="B94" s="0" t="str">
-        <v>1005288</v>
+        <v>1005289</v>
       </c>
     </row>
     <row r="95" spans="1:2" customFormat="false">
       <c r="A95" s="0" t="str">
-        <v>52095</v>
+        <v>52096</v>
       </c>
       <c r="B95" s="0" t="str">
-        <v>1005289</v>
+        <v>1005290</v>
       </c>
     </row>
     <row r="96" spans="1:2" customFormat="false">
       <c r="A96" s="0" t="str">
-        <v>52096</v>
+        <v>52057</v>
       </c>
       <c r="B96" s="0" t="str">
-        <v>1005290</v>
+        <v>1005251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed single locker bug
</commit_message>
<xml_diff>
--- a/lib/CVHS Locker Template and Guide.xlsx
+++ b/lib/CVHS Locker Template and Guide.xlsx
@@ -39238,7 +39238,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <dimension ref="A1:B221"/>
+  <dimension ref="A1:B222"/>
   <sheetData>
     <row r="1" spans="1:2" customFormat="false">
       <c r="A1" s="0" t="str">
@@ -41006,6 +41006,14 @@
       </c>
       <c r="B221" s="0" t="str">
         <v>1004048</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" customFormat="false">
+      <c r="A222" s="0" t="str">
+        <v>6112</v>
+      </c>
+      <c r="B222" s="0" t="str">
+        <v>1004221</v>
       </c>
     </row>
   </sheetData>
@@ -41014,7 +41022,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <dimension ref="A1:B225"/>
+  <dimension ref="A1:B224"/>
   <sheetData>
     <row r="1" spans="1:2" customFormat="false">
       <c r="A1" s="0" t="str">
@@ -42394,425 +42402,417 @@
     </row>
     <row r="173" spans="1:2" customFormat="false">
       <c r="A173" s="0" t="str">
-        <v>6112</v>
+        <v>6113</v>
       </c>
       <c r="B173" s="0" t="str">
-        <v>1004221</v>
+        <v>1004222</v>
       </c>
     </row>
     <row r="174" spans="1:2" customFormat="false">
       <c r="A174" s="0" t="str">
-        <v>6113</v>
+        <v>6114</v>
       </c>
       <c r="B174" s="0" t="str">
-        <v>1004222</v>
+        <v>1004223</v>
       </c>
     </row>
     <row r="175" spans="1:2" customFormat="false">
       <c r="A175" s="0" t="str">
-        <v>6114</v>
+        <v>6115</v>
       </c>
       <c r="B175" s="0" t="str">
-        <v>1004223</v>
+        <v>1004224</v>
       </c>
     </row>
     <row r="176" spans="1:2" customFormat="false">
       <c r="A176" s="0" t="str">
-        <v>6115</v>
+        <v>6116</v>
       </c>
       <c r="B176" s="0" t="str">
-        <v>1004224</v>
+        <v>1004225</v>
       </c>
     </row>
     <row r="177" spans="1:2" customFormat="false">
       <c r="A177" s="0" t="str">
-        <v>6116</v>
+        <v>6117</v>
       </c>
       <c r="B177" s="0" t="str">
-        <v>1004225</v>
+        <v>1004226</v>
       </c>
     </row>
     <row r="178" spans="1:2" customFormat="false">
       <c r="A178" s="0" t="str">
-        <v>6117</v>
+        <v>6118</v>
       </c>
       <c r="B178" s="0" t="str">
-        <v>1004226</v>
+        <v>1004227</v>
       </c>
     </row>
     <row r="179" spans="1:2" customFormat="false">
       <c r="A179" s="0" t="str">
-        <v>6118</v>
+        <v>6119</v>
       </c>
       <c r="B179" s="0" t="str">
-        <v>1004227</v>
+        <v>1004228</v>
       </c>
     </row>
     <row r="180" spans="1:2" customFormat="false">
       <c r="A180" s="0" t="str">
-        <v>6119</v>
+        <v>6120</v>
       </c>
       <c r="B180" s="0" t="str">
-        <v>1004228</v>
+        <v>1004229</v>
       </c>
     </row>
     <row r="181" spans="1:2" customFormat="false">
       <c r="A181" s="0" t="str">
-        <v>6120</v>
+        <v>6121</v>
       </c>
       <c r="B181" s="0" t="str">
-        <v>1004229</v>
+        <v>1004230</v>
       </c>
     </row>
     <row r="182" spans="1:2" customFormat="false">
       <c r="A182" s="0" t="str">
-        <v>6121</v>
+        <v>6122</v>
       </c>
       <c r="B182" s="0" t="str">
-        <v>1004230</v>
+        <v>1004231</v>
       </c>
     </row>
     <row r="183" spans="1:2" customFormat="false">
       <c r="A183" s="0" t="str">
-        <v>6122</v>
+        <v>6123</v>
       </c>
       <c r="B183" s="0" t="str">
-        <v>1004231</v>
+        <v>1004232</v>
       </c>
     </row>
     <row r="184" spans="1:2" customFormat="false">
       <c r="A184" s="0" t="str">
-        <v>6123</v>
+        <v>6124</v>
       </c>
       <c r="B184" s="0" t="str">
-        <v>1004232</v>
+        <v>1004233</v>
       </c>
     </row>
     <row r="185" spans="1:2" customFormat="false">
       <c r="A185" s="0" t="str">
-        <v>6124</v>
+        <v>6125</v>
       </c>
       <c r="B185" s="0" t="str">
-        <v>1004233</v>
+        <v>1004234</v>
       </c>
     </row>
     <row r="186" spans="1:2" customFormat="false">
       <c r="A186" s="0" t="str">
-        <v>6125</v>
+        <v>6126</v>
       </c>
       <c r="B186" s="0" t="str">
-        <v>1004234</v>
+        <v>1004235</v>
       </c>
     </row>
     <row r="187" spans="1:2" customFormat="false">
       <c r="A187" s="0" t="str">
-        <v>6126</v>
+        <v>6127</v>
       </c>
       <c r="B187" s="0" t="str">
-        <v>1004235</v>
+        <v>1004236</v>
       </c>
     </row>
     <row r="188" spans="1:2" customFormat="false">
       <c r="A188" s="0" t="str">
-        <v>6127</v>
+        <v>6128</v>
       </c>
       <c r="B188" s="0" t="str">
-        <v>1004236</v>
+        <v>1004237</v>
       </c>
     </row>
     <row r="189" spans="1:2" customFormat="false">
       <c r="A189" s="0" t="str">
-        <v>6128</v>
+        <v>6129</v>
       </c>
       <c r="B189" s="0" t="str">
-        <v>1004237</v>
+        <v>1004238</v>
       </c>
     </row>
     <row r="190" spans="1:2" customFormat="false">
       <c r="A190" s="0" t="str">
-        <v>6129</v>
+        <v>6130</v>
       </c>
       <c r="B190" s="0" t="str">
-        <v>1004238</v>
+        <v>1004239</v>
       </c>
     </row>
     <row r="191" spans="1:2" customFormat="false">
       <c r="A191" s="0" t="str">
-        <v>6130</v>
+        <v>6131</v>
       </c>
       <c r="B191" s="0" t="str">
-        <v>1004239</v>
+        <v>1004240</v>
       </c>
     </row>
     <row r="192" spans="1:2" customFormat="false">
       <c r="A192" s="0" t="str">
-        <v>6131</v>
+        <v>6132</v>
       </c>
       <c r="B192" s="0" t="str">
-        <v>1004240</v>
+        <v>1004241</v>
       </c>
     </row>
     <row r="193" spans="1:2" customFormat="false">
       <c r="A193" s="0" t="str">
-        <v>6132</v>
+        <v>6133</v>
       </c>
       <c r="B193" s="0" t="str">
-        <v>1004241</v>
+        <v>1004242</v>
       </c>
     </row>
     <row r="194" spans="1:2" customFormat="false">
       <c r="A194" s="0" t="str">
-        <v>6133</v>
+        <v>6134</v>
       </c>
       <c r="B194" s="0" t="str">
-        <v>1004242</v>
+        <v>1004243</v>
       </c>
     </row>
     <row r="195" spans="1:2" customFormat="false">
       <c r="A195" s="0" t="str">
-        <v>6134</v>
+        <v>6135</v>
       </c>
       <c r="B195" s="0" t="str">
-        <v>1004243</v>
+        <v>1004244</v>
       </c>
     </row>
     <row r="196" spans="1:2" customFormat="false">
       <c r="A196" s="0" t="str">
-        <v>6135</v>
+        <v>6136</v>
       </c>
       <c r="B196" s="0" t="str">
-        <v>1004244</v>
+        <v>1004245</v>
       </c>
     </row>
     <row r="197" spans="1:2" customFormat="false">
       <c r="A197" s="0" t="str">
-        <v>6136</v>
+        <v>6137</v>
       </c>
       <c r="B197" s="0" t="str">
-        <v>1004245</v>
+        <v>1004246</v>
       </c>
     </row>
     <row r="198" spans="1:2" customFormat="false">
       <c r="A198" s="0" t="str">
-        <v>6137</v>
+        <v>6138</v>
       </c>
       <c r="B198" s="0" t="str">
-        <v>1004246</v>
+        <v>1004247</v>
       </c>
     </row>
     <row r="199" spans="1:2" customFormat="false">
       <c r="A199" s="0" t="str">
-        <v>6138</v>
+        <v>6139</v>
       </c>
       <c r="B199" s="0" t="str">
-        <v>1004247</v>
+        <v>1004248</v>
       </c>
     </row>
     <row r="200" spans="1:2" customFormat="false">
       <c r="A200" s="0" t="str">
-        <v>6139</v>
+        <v>6140</v>
       </c>
       <c r="B200" s="0" t="str">
-        <v>1004248</v>
+        <v>1004249</v>
       </c>
     </row>
     <row r="201" spans="1:2" customFormat="false">
       <c r="A201" s="0" t="str">
-        <v>6140</v>
+        <v>6141</v>
       </c>
       <c r="B201" s="0" t="str">
-        <v>1004249</v>
+        <v>1004250</v>
       </c>
     </row>
     <row r="202" spans="1:2" customFormat="false">
       <c r="A202" s="0" t="str">
-        <v>6141</v>
+        <v>6142</v>
       </c>
       <c r="B202" s="0" t="str">
-        <v>1004250</v>
+        <v>1004251</v>
       </c>
     </row>
     <row r="203" spans="1:2" customFormat="false">
       <c r="A203" s="0" t="str">
-        <v>6142</v>
+        <v>6143</v>
       </c>
       <c r="B203" s="0" t="str">
-        <v>1004251</v>
+        <v>1004252</v>
       </c>
     </row>
     <row r="204" spans="1:2" customFormat="false">
       <c r="A204" s="0" t="str">
-        <v>6143</v>
+        <v>6144</v>
       </c>
       <c r="B204" s="0" t="str">
-        <v>1004252</v>
+        <v>1004253</v>
       </c>
     </row>
     <row r="205" spans="1:2" customFormat="false">
       <c r="A205" s="0" t="str">
-        <v>6144</v>
+        <v>6145</v>
       </c>
       <c r="B205" s="0" t="str">
-        <v>1004253</v>
+        <v>1004254</v>
       </c>
     </row>
     <row r="206" spans="1:2" customFormat="false">
       <c r="A206" s="0" t="str">
-        <v>6145</v>
+        <v>6146</v>
       </c>
       <c r="B206" s="0" t="str">
-        <v>1004254</v>
+        <v>1004255</v>
       </c>
     </row>
     <row r="207" spans="1:2" customFormat="false">
       <c r="A207" s="0" t="str">
-        <v>6146</v>
+        <v>6147</v>
       </c>
       <c r="B207" s="0" t="str">
-        <v>1004255</v>
+        <v>1004256</v>
       </c>
     </row>
     <row r="208" spans="1:2" customFormat="false">
       <c r="A208" s="0" t="str">
-        <v>6147</v>
+        <v>6148</v>
       </c>
       <c r="B208" s="0" t="str">
-        <v>1004256</v>
+        <v>1004257</v>
       </c>
     </row>
     <row r="209" spans="1:2" customFormat="false">
       <c r="A209" s="0" t="str">
-        <v>6148</v>
+        <v>6149</v>
       </c>
       <c r="B209" s="0" t="str">
-        <v>1004257</v>
+        <v>1004258</v>
       </c>
     </row>
     <row r="210" spans="1:2" customFormat="false">
       <c r="A210" s="0" t="str">
-        <v>6149</v>
+        <v>6150</v>
       </c>
       <c r="B210" s="0" t="str">
-        <v>1004258</v>
+        <v>1004259</v>
       </c>
     </row>
     <row r="211" spans="1:2" customFormat="false">
       <c r="A211" s="0" t="str">
-        <v>6150</v>
+        <v>6151</v>
       </c>
       <c r="B211" s="0" t="str">
-        <v>1004259</v>
+        <v>1004260</v>
       </c>
     </row>
     <row r="212" spans="1:2" customFormat="false">
       <c r="A212" s="0" t="str">
-        <v>6151</v>
+        <v>6152</v>
       </c>
       <c r="B212" s="0" t="str">
-        <v>1004260</v>
+        <v>1004261</v>
       </c>
     </row>
     <row r="213" spans="1:2" customFormat="false">
       <c r="A213" s="0" t="str">
-        <v>6152</v>
+        <v>6153</v>
       </c>
       <c r="B213" s="0" t="str">
-        <v>1004261</v>
+        <v>1004262</v>
       </c>
     </row>
     <row r="214" spans="1:2" customFormat="false">
       <c r="A214" s="0" t="str">
-        <v>6153</v>
+        <v>6154</v>
       </c>
       <c r="B214" s="0" t="str">
-        <v>1004262</v>
+        <v>1004263</v>
       </c>
     </row>
     <row r="215" spans="1:2" customFormat="false">
       <c r="A215" s="0" t="str">
-        <v>6154</v>
+        <v>6155</v>
       </c>
       <c r="B215" s="0" t="str">
-        <v>1004263</v>
+        <v>1004264</v>
       </c>
     </row>
     <row r="216" spans="1:2" customFormat="false">
       <c r="A216" s="0" t="str">
-        <v>6155</v>
+        <v>6156</v>
       </c>
       <c r="B216" s="0" t="str">
-        <v>1004264</v>
+        <v>1004265</v>
       </c>
     </row>
     <row r="217" spans="1:2" customFormat="false">
       <c r="A217" s="0" t="str">
-        <v>6156</v>
+        <v>6157</v>
       </c>
       <c r="B217" s="0" t="str">
-        <v>1004265</v>
+        <v>1004266</v>
       </c>
     </row>
     <row r="218" spans="1:2" customFormat="false">
       <c r="A218" s="0" t="str">
-        <v>6157</v>
+        <v>6158</v>
       </c>
       <c r="B218" s="0" t="str">
-        <v>1004266</v>
+        <v>1004267</v>
       </c>
     </row>
     <row r="219" spans="1:2" customFormat="false">
       <c r="A219" s="0" t="str">
-        <v>6158</v>
+        <v>6159</v>
       </c>
       <c r="B219" s="0" t="str">
-        <v>1004267</v>
+        <v>1004268</v>
       </c>
     </row>
     <row r="220" spans="1:2" customFormat="false">
       <c r="A220" s="0" t="str">
-        <v>6159</v>
+        <v>6160</v>
       </c>
       <c r="B220" s="0" t="str">
-        <v>1004268</v>
+        <v>1004269</v>
       </c>
     </row>
     <row r="221" spans="1:2" customFormat="false">
       <c r="A221" s="0" t="str">
-        <v>6160</v>
+        <v>6161</v>
       </c>
       <c r="B221" s="0" t="str">
-        <v>1004269</v>
+        <v>1004270</v>
       </c>
     </row>
     <row r="222" spans="1:2" customFormat="false">
       <c r="A222" s="0" t="str">
-        <v>6161</v>
+        <v>6162</v>
       </c>
       <c r="B222" s="0" t="str">
-        <v>1004270</v>
+        <v>1004271</v>
       </c>
     </row>
     <row r="223" spans="1:2" customFormat="false">
       <c r="A223" s="0" t="str">
-        <v>6162</v>
+        <v>6163</v>
       </c>
       <c r="B223" s="0" t="str">
-        <v>1004271</v>
+        <v>1004272</v>
       </c>
     </row>
     <row r="224" spans="1:2" customFormat="false">
       <c r="A224" s="0" t="str">
-        <v>6163</v>
+        <v>6164</v>
       </c>
       <c r="B224" s="0" t="str">
-        <v>1004272</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" customFormat="false">
-      <c r="A225" s="0" t="str">
-        <v>6164</v>
-      </c>
-      <c r="B225" s="0" t="str">
         <v>1004273</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix restriction bug and required
</commit_message>
<xml_diff>
--- a/lib/CVHS Locker Template and Guide.xlsx
+++ b/lib/CVHS Locker Template and Guide.xlsx
@@ -34734,7 +34734,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <dimension ref="A1:B168"/>
+  <dimension ref="A1:B167"/>
   <sheetData>
     <row r="1" spans="1:2" customFormat="false">
       <c r="A1" s="0" t="str">
@@ -34930,1153 +34930,1145 @@
     </row>
     <row r="25" spans="1:2" customFormat="false">
       <c r="A25" s="0" t="str">
-        <v>53025</v>
+        <v>53026</v>
       </c>
       <c r="B25" s="0" t="str">
-        <v>1005315</v>
+        <v>1005316</v>
       </c>
     </row>
     <row r="26" spans="1:2" customFormat="false">
       <c r="A26" s="0" t="str">
-        <v>53026</v>
+        <v>53027</v>
       </c>
       <c r="B26" s="0" t="str">
-        <v>1005316</v>
+        <v>1005317</v>
       </c>
     </row>
     <row r="27" spans="1:2" customFormat="false">
       <c r="A27" s="0" t="str">
-        <v>53027</v>
+        <v>53028</v>
       </c>
       <c r="B27" s="0" t="str">
-        <v>1005317</v>
+        <v>1005318</v>
       </c>
     </row>
     <row r="28" spans="1:2" customFormat="false">
       <c r="A28" s="0" t="str">
-        <v>53028</v>
+        <v>53029</v>
       </c>
       <c r="B28" s="0" t="str">
-        <v>1005318</v>
+        <v>1005319</v>
       </c>
     </row>
     <row r="29" spans="1:2" customFormat="false">
       <c r="A29" s="0" t="str">
-        <v>53029</v>
+        <v>53030</v>
       </c>
       <c r="B29" s="0" t="str">
-        <v>1005319</v>
+        <v>1005320</v>
       </c>
     </row>
     <row r="30" spans="1:2" customFormat="false">
       <c r="A30" s="0" t="str">
-        <v>53030</v>
+        <v>53031</v>
       </c>
       <c r="B30" s="0" t="str">
-        <v>1005320</v>
+        <v>1005321</v>
       </c>
     </row>
     <row r="31" spans="1:2" customFormat="false">
       <c r="A31" s="0" t="str">
-        <v>53031</v>
+        <v>53032</v>
       </c>
       <c r="B31" s="0" t="str">
-        <v>1005321</v>
+        <v>1005322</v>
       </c>
     </row>
     <row r="32" spans="1:2" customFormat="false">
       <c r="A32" s="0" t="str">
-        <v>53032</v>
+        <v>53033</v>
       </c>
       <c r="B32" s="0" t="str">
-        <v>1005322</v>
+        <v>1005323</v>
       </c>
     </row>
     <row r="33" spans="1:2" customFormat="false">
       <c r="A33" s="0" t="str">
-        <v>53033</v>
+        <v>53034</v>
       </c>
       <c r="B33" s="0" t="str">
-        <v>1005323</v>
+        <v>1005324</v>
       </c>
     </row>
     <row r="34" spans="1:2" customFormat="false">
       <c r="A34" s="0" t="str">
-        <v>53034</v>
+        <v>53035</v>
       </c>
       <c r="B34" s="0" t="str">
-        <v>1005324</v>
+        <v>1005325</v>
       </c>
     </row>
     <row r="35" spans="1:2" customFormat="false">
       <c r="A35" s="0" t="str">
-        <v>53035</v>
+        <v>53036</v>
       </c>
       <c r="B35" s="0" t="str">
-        <v>1005325</v>
+        <v>1005326</v>
       </c>
     </row>
     <row r="36" spans="1:2" customFormat="false">
       <c r="A36" s="0" t="str">
-        <v>53036</v>
+        <v>53037</v>
       </c>
       <c r="B36" s="0" t="str">
-        <v>1005326</v>
+        <v>1005327</v>
       </c>
     </row>
     <row r="37" spans="1:2" customFormat="false">
       <c r="A37" s="0" t="str">
-        <v>53037</v>
+        <v>53038</v>
       </c>
       <c r="B37" s="0" t="str">
-        <v>1005327</v>
+        <v>1005328</v>
       </c>
     </row>
     <row r="38" spans="1:2" customFormat="false">
       <c r="A38" s="0" t="str">
-        <v>53038</v>
+        <v>53039</v>
       </c>
       <c r="B38" s="0" t="str">
-        <v>1005328</v>
+        <v>1005329</v>
       </c>
     </row>
     <row r="39" spans="1:2" customFormat="false">
       <c r="A39" s="0" t="str">
-        <v>53039</v>
+        <v>53040</v>
       </c>
       <c r="B39" s="0" t="str">
-        <v>1005329</v>
+        <v>1005330</v>
       </c>
     </row>
     <row r="40" spans="1:2" customFormat="false">
       <c r="A40" s="0" t="str">
-        <v>53040</v>
+        <v>53041</v>
       </c>
       <c r="B40" s="0" t="str">
-        <v>1005330</v>
+        <v>1005331</v>
       </c>
     </row>
     <row r="41" spans="1:2" customFormat="false">
       <c r="A41" s="0" t="str">
-        <v>53041</v>
+        <v>53042</v>
       </c>
       <c r="B41" s="0" t="str">
-        <v>1005331</v>
+        <v>1005332</v>
       </c>
     </row>
     <row r="42" spans="1:2" customFormat="false">
       <c r="A42" s="0" t="str">
-        <v>53042</v>
+        <v>53043</v>
       </c>
       <c r="B42" s="0" t="str">
-        <v>1005332</v>
+        <v>1005333</v>
       </c>
     </row>
     <row r="43" spans="1:2" customFormat="false">
       <c r="A43" s="0" t="str">
-        <v>53043</v>
+        <v>53044</v>
       </c>
       <c r="B43" s="0" t="str">
-        <v>1005333</v>
+        <v>1005334</v>
       </c>
     </row>
     <row r="44" spans="1:2" customFormat="false">
       <c r="A44" s="0" t="str">
-        <v>53044</v>
+        <v>53045</v>
       </c>
       <c r="B44" s="0" t="str">
-        <v>1005334</v>
+        <v>1005335</v>
       </c>
     </row>
     <row r="45" spans="1:2" customFormat="false">
       <c r="A45" s="0" t="str">
-        <v>53045</v>
+        <v>53046</v>
       </c>
       <c r="B45" s="0" t="str">
-        <v>1005335</v>
+        <v>1005336</v>
       </c>
     </row>
     <row r="46" spans="1:2" customFormat="false">
       <c r="A46" s="0" t="str">
-        <v>53046</v>
+        <v>53047</v>
       </c>
       <c r="B46" s="0" t="str">
-        <v>1005336</v>
+        <v>1005337</v>
       </c>
     </row>
     <row r="47" spans="1:2" customFormat="false">
       <c r="A47" s="0" t="str">
-        <v>53047</v>
+        <v>53048</v>
       </c>
       <c r="B47" s="0" t="str">
-        <v>1005337</v>
+        <v>1005338</v>
       </c>
     </row>
     <row r="48" spans="1:2" customFormat="false">
       <c r="A48" s="0" t="str">
-        <v>53048</v>
+        <v>53049</v>
       </c>
       <c r="B48" s="0" t="str">
-        <v>1005338</v>
+        <v>1005339</v>
       </c>
     </row>
     <row r="49" spans="1:2" customFormat="false">
       <c r="A49" s="0" t="str">
-        <v>53049</v>
+        <v>53050</v>
       </c>
       <c r="B49" s="0" t="str">
-        <v>1005339</v>
+        <v>1005340</v>
       </c>
     </row>
     <row r="50" spans="1:2" customFormat="false">
       <c r="A50" s="0" t="str">
-        <v>53050</v>
+        <v>53051</v>
       </c>
       <c r="B50" s="0" t="str">
-        <v>1005340</v>
+        <v>1005341</v>
       </c>
     </row>
     <row r="51" spans="1:2" customFormat="false">
       <c r="A51" s="0" t="str">
-        <v>53051</v>
+        <v>53052</v>
       </c>
       <c r="B51" s="0" t="str">
-        <v>1005341</v>
+        <v>1005342</v>
       </c>
     </row>
     <row r="52" spans="1:2" customFormat="false">
       <c r="A52" s="0" t="str">
-        <v>53052</v>
+        <v>53053</v>
       </c>
       <c r="B52" s="0" t="str">
-        <v>1005342</v>
+        <v>1005343</v>
       </c>
     </row>
     <row r="53" spans="1:2" customFormat="false">
       <c r="A53" s="0" t="str">
-        <v>53053</v>
+        <v>53054</v>
       </c>
       <c r="B53" s="0" t="str">
-        <v>1005343</v>
+        <v>1005344</v>
       </c>
     </row>
     <row r="54" spans="1:2" customFormat="false">
       <c r="A54" s="0" t="str">
-        <v>53054</v>
+        <v>53055</v>
       </c>
       <c r="B54" s="0" t="str">
-        <v>1005344</v>
+        <v>1005345</v>
       </c>
     </row>
     <row r="55" spans="1:2" customFormat="false">
       <c r="A55" s="0" t="str">
-        <v>53055</v>
+        <v>53056</v>
       </c>
       <c r="B55" s="0" t="str">
-        <v>1005345</v>
+        <v>1005346</v>
       </c>
     </row>
     <row r="56" spans="1:2" customFormat="false">
       <c r="A56" s="0" t="str">
-        <v>53056</v>
+        <v>53057</v>
       </c>
       <c r="B56" s="0" t="str">
-        <v>1005346</v>
+        <v>1005347</v>
       </c>
     </row>
     <row r="57" spans="1:2" customFormat="false">
       <c r="A57" s="0" t="str">
-        <v>53057</v>
+        <v>53058</v>
       </c>
       <c r="B57" s="0" t="str">
-        <v>1005347</v>
+        <v>1005348</v>
       </c>
     </row>
     <row r="58" spans="1:2" customFormat="false">
       <c r="A58" s="0" t="str">
-        <v>53058</v>
+        <v>53059</v>
       </c>
       <c r="B58" s="0" t="str">
-        <v>1005348</v>
+        <v>1005349</v>
       </c>
     </row>
     <row r="59" spans="1:2" customFormat="false">
       <c r="A59" s="0" t="str">
-        <v>53059</v>
+        <v>53060</v>
       </c>
       <c r="B59" s="0" t="str">
-        <v>1005349</v>
+        <v>1005350</v>
       </c>
     </row>
     <row r="60" spans="1:2" customFormat="false">
       <c r="A60" s="0" t="str">
-        <v>53060</v>
+        <v>53061</v>
       </c>
       <c r="B60" s="0" t="str">
-        <v>1005350</v>
+        <v>1005351</v>
       </c>
     </row>
     <row r="61" spans="1:2" customFormat="false">
       <c r="A61" s="0" t="str">
-        <v>53061</v>
+        <v>53062</v>
       </c>
       <c r="B61" s="0" t="str">
-        <v>1005351</v>
+        <v>1005352</v>
       </c>
     </row>
     <row r="62" spans="1:2" customFormat="false">
       <c r="A62" s="0" t="str">
-        <v>53062</v>
+        <v>53063</v>
       </c>
       <c r="B62" s="0" t="str">
-        <v>1005352</v>
+        <v>1005353</v>
       </c>
     </row>
     <row r="63" spans="1:2" customFormat="false">
       <c r="A63" s="0" t="str">
-        <v>53063</v>
+        <v>53064</v>
       </c>
       <c r="B63" s="0" t="str">
-        <v>1005353</v>
+        <v>1005354</v>
       </c>
     </row>
     <row r="64" spans="1:2" customFormat="false">
       <c r="A64" s="0" t="str">
-        <v>53064</v>
+        <v>53065</v>
       </c>
       <c r="B64" s="0" t="str">
-        <v>1005354</v>
+        <v>1005355</v>
       </c>
     </row>
     <row r="65" spans="1:2" customFormat="false">
       <c r="A65" s="0" t="str">
-        <v>53065</v>
+        <v>53066</v>
       </c>
       <c r="B65" s="0" t="str">
-        <v>1005355</v>
+        <v>1005356</v>
       </c>
     </row>
     <row r="66" spans="1:2" customFormat="false">
       <c r="A66" s="0" t="str">
-        <v>53066</v>
+        <v>53067</v>
       </c>
       <c r="B66" s="0" t="str">
-        <v>1005356</v>
+        <v>1005357</v>
       </c>
     </row>
     <row r="67" spans="1:2" customFormat="false">
       <c r="A67" s="0" t="str">
-        <v>53067</v>
+        <v>53068</v>
       </c>
       <c r="B67" s="0" t="str">
-        <v>1005357</v>
+        <v>1005358</v>
       </c>
     </row>
     <row r="68" spans="1:2" customFormat="false">
       <c r="A68" s="0" t="str">
-        <v>53068</v>
+        <v>53069</v>
       </c>
       <c r="B68" s="0" t="str">
-        <v>1005358</v>
+        <v>1005359</v>
       </c>
     </row>
     <row r="69" spans="1:2" customFormat="false">
       <c r="A69" s="0" t="str">
-        <v>53069</v>
+        <v>53070</v>
       </c>
       <c r="B69" s="0" t="str">
-        <v>1005359</v>
+        <v>1005360</v>
       </c>
     </row>
     <row r="70" spans="1:2" customFormat="false">
       <c r="A70" s="0" t="str">
-        <v>53070</v>
+        <v>53071</v>
       </c>
       <c r="B70" s="0" t="str">
-        <v>1005360</v>
+        <v>1005361</v>
       </c>
     </row>
     <row r="71" spans="1:2" customFormat="false">
       <c r="A71" s="0" t="str">
-        <v>53071</v>
+        <v>53072</v>
       </c>
       <c r="B71" s="0" t="str">
-        <v>1005361</v>
+        <v>1005362</v>
       </c>
     </row>
     <row r="72" spans="1:2" customFormat="false">
       <c r="A72" s="0" t="str">
-        <v>53072</v>
+        <v>53073</v>
       </c>
       <c r="B72" s="0" t="str">
-        <v>1005362</v>
+        <v>1005363</v>
       </c>
     </row>
     <row r="73" spans="1:2" customFormat="false">
       <c r="A73" s="0" t="str">
-        <v>53073</v>
+        <v>53074</v>
       </c>
       <c r="B73" s="0" t="str">
-        <v>1005363</v>
+        <v>1005364</v>
       </c>
     </row>
     <row r="74" spans="1:2" customFormat="false">
       <c r="A74" s="0" t="str">
-        <v>53074</v>
+        <v>53075</v>
       </c>
       <c r="B74" s="0" t="str">
-        <v>1005364</v>
+        <v>1005365</v>
       </c>
     </row>
     <row r="75" spans="1:2" customFormat="false">
       <c r="A75" s="0" t="str">
-        <v>53075</v>
+        <v>53076</v>
       </c>
       <c r="B75" s="0" t="str">
-        <v>1005365</v>
+        <v>1005366</v>
       </c>
     </row>
     <row r="76" spans="1:2" customFormat="false">
       <c r="A76" s="0" t="str">
-        <v>53076</v>
+        <v>53077</v>
       </c>
       <c r="B76" s="0" t="str">
-        <v>1005366</v>
+        <v>1005367</v>
       </c>
     </row>
     <row r="77" spans="1:2" customFormat="false">
       <c r="A77" s="0" t="str">
-        <v>53077</v>
+        <v>53078</v>
       </c>
       <c r="B77" s="0" t="str">
-        <v>1005367</v>
+        <v>1005368</v>
       </c>
     </row>
     <row r="78" spans="1:2" customFormat="false">
       <c r="A78" s="0" t="str">
-        <v>53078</v>
+        <v>53079</v>
       </c>
       <c r="B78" s="0" t="str">
-        <v>1005368</v>
+        <v>1005369</v>
       </c>
     </row>
     <row r="79" spans="1:2" customFormat="false">
       <c r="A79" s="0" t="str">
-        <v>53079</v>
+        <v>53080</v>
       </c>
       <c r="B79" s="0" t="str">
-        <v>1005369</v>
+        <v>1005370</v>
       </c>
     </row>
     <row r="80" spans="1:2" customFormat="false">
       <c r="A80" s="0" t="str">
-        <v>53080</v>
+        <v>53081</v>
       </c>
       <c r="B80" s="0" t="str">
-        <v>1005370</v>
+        <v>1005371</v>
       </c>
     </row>
     <row r="81" spans="1:2" customFormat="false">
       <c r="A81" s="0" t="str">
-        <v>53081</v>
+        <v>53082</v>
       </c>
       <c r="B81" s="0" t="str">
-        <v>1005371</v>
+        <v>1005372</v>
       </c>
     </row>
     <row r="82" spans="1:2" customFormat="false">
       <c r="A82" s="0" t="str">
-        <v>53082</v>
+        <v>53083</v>
       </c>
       <c r="B82" s="0" t="str">
-        <v>1005372</v>
+        <v>1005373</v>
       </c>
     </row>
     <row r="83" spans="1:2" customFormat="false">
       <c r="A83" s="0" t="str">
-        <v>53083</v>
+        <v>53084</v>
       </c>
       <c r="B83" s="0" t="str">
-        <v>1005373</v>
+        <v>1005374</v>
       </c>
     </row>
     <row r="84" spans="1:2" customFormat="false">
       <c r="A84" s="0" t="str">
-        <v>53084</v>
+        <v>53085</v>
       </c>
       <c r="B84" s="0" t="str">
-        <v>1005374</v>
+        <v>1005375</v>
       </c>
     </row>
     <row r="85" spans="1:2" customFormat="false">
       <c r="A85" s="0" t="str">
-        <v>53085</v>
+        <v>53086</v>
       </c>
       <c r="B85" s="0" t="str">
-        <v>1005375</v>
+        <v>1005376</v>
       </c>
     </row>
     <row r="86" spans="1:2" customFormat="false">
       <c r="A86" s="0" t="str">
-        <v>53086</v>
+        <v>53087</v>
       </c>
       <c r="B86" s="0" t="str">
-        <v>1005376</v>
+        <v>1005377</v>
       </c>
     </row>
     <row r="87" spans="1:2" customFormat="false">
       <c r="A87" s="0" t="str">
-        <v>53087</v>
+        <v>53088</v>
       </c>
       <c r="B87" s="0" t="str">
-        <v>1005377</v>
+        <v>1005378</v>
       </c>
     </row>
     <row r="88" spans="1:2" customFormat="false">
       <c r="A88" s="0" t="str">
-        <v>53088</v>
+        <v>53089</v>
       </c>
       <c r="B88" s="0" t="str">
-        <v>1005378</v>
+        <v>1005379</v>
       </c>
     </row>
     <row r="89" spans="1:2" customFormat="false">
       <c r="A89" s="0" t="str">
-        <v>53089</v>
+        <v>53090</v>
       </c>
       <c r="B89" s="0" t="str">
-        <v>1005379</v>
+        <v>1005380</v>
       </c>
     </row>
     <row r="90" spans="1:2" customFormat="false">
       <c r="A90" s="0" t="str">
-        <v>53090</v>
+        <v>53091</v>
       </c>
       <c r="B90" s="0" t="str">
-        <v>1005380</v>
+        <v>1005381</v>
       </c>
     </row>
     <row r="91" spans="1:2" customFormat="false">
       <c r="A91" s="0" t="str">
-        <v>53091</v>
+        <v>53092</v>
       </c>
       <c r="B91" s="0" t="str">
-        <v>1005381</v>
+        <v>1005382</v>
       </c>
     </row>
     <row r="92" spans="1:2" customFormat="false">
       <c r="A92" s="0" t="str">
-        <v>53092</v>
+        <v>53093</v>
       </c>
       <c r="B92" s="0" t="str">
-        <v>1005382</v>
+        <v>1005383</v>
       </c>
     </row>
     <row r="93" spans="1:2" customFormat="false">
       <c r="A93" s="0" t="str">
-        <v>53093</v>
+        <v>53094</v>
       </c>
       <c r="B93" s="0" t="str">
-        <v>1005383</v>
+        <v>1005384</v>
       </c>
     </row>
     <row r="94" spans="1:2" customFormat="false">
       <c r="A94" s="0" t="str">
-        <v>53094</v>
+        <v>53095</v>
       </c>
       <c r="B94" s="0" t="str">
-        <v>1005384</v>
+        <v>1005385</v>
       </c>
     </row>
     <row r="95" spans="1:2" customFormat="false">
       <c r="A95" s="0" t="str">
-        <v>53095</v>
+        <v>53096</v>
       </c>
       <c r="B95" s="0" t="str">
-        <v>1005385</v>
+        <v>1005386</v>
       </c>
     </row>
     <row r="96" spans="1:2" customFormat="false">
       <c r="A96" s="0" t="str">
-        <v>53096</v>
+        <v>53097</v>
       </c>
       <c r="B96" s="0" t="str">
-        <v>1005386</v>
+        <v>1005387</v>
       </c>
     </row>
     <row r="97" spans="1:2" customFormat="false">
       <c r="A97" s="0" t="str">
-        <v>53097</v>
+        <v>53098</v>
       </c>
       <c r="B97" s="0" t="str">
-        <v>1005387</v>
+        <v>1005388</v>
       </c>
     </row>
     <row r="98" spans="1:2" customFormat="false">
       <c r="A98" s="0" t="str">
-        <v>53098</v>
+        <v>53099</v>
       </c>
       <c r="B98" s="0" t="str">
-        <v>1005388</v>
+        <v>1005389</v>
       </c>
     </row>
     <row r="99" spans="1:2" customFormat="false">
       <c r="A99" s="0" t="str">
-        <v>53099</v>
+        <v>53100</v>
       </c>
       <c r="B99" s="0" t="str">
-        <v>1005389</v>
+        <v>1005390</v>
       </c>
     </row>
     <row r="100" spans="1:2" customFormat="false">
       <c r="A100" s="0" t="str">
-        <v>53100</v>
+        <v>53101</v>
       </c>
       <c r="B100" s="0" t="str">
-        <v>1005390</v>
+        <v>1005391</v>
       </c>
     </row>
     <row r="101" spans="1:2" customFormat="false">
       <c r="A101" s="0" t="str">
-        <v>53101</v>
+        <v>53102</v>
       </c>
       <c r="B101" s="0" t="str">
-        <v>1005391</v>
+        <v>1005392</v>
       </c>
     </row>
     <row r="102" spans="1:2" customFormat="false">
       <c r="A102" s="0" t="str">
-        <v>53102</v>
+        <v>53103</v>
       </c>
       <c r="B102" s="0" t="str">
-        <v>1005392</v>
+        <v>1005393</v>
       </c>
     </row>
     <row r="103" spans="1:2" customFormat="false">
       <c r="A103" s="0" t="str">
-        <v>53103</v>
+        <v>53104</v>
       </c>
       <c r="B103" s="0" t="str">
-        <v>1005393</v>
+        <v>1005394</v>
       </c>
     </row>
     <row r="104" spans="1:2" customFormat="false">
       <c r="A104" s="0" t="str">
-        <v>53104</v>
+        <v>53105</v>
       </c>
       <c r="B104" s="0" t="str">
-        <v>1005394</v>
+        <v>1005395</v>
       </c>
     </row>
     <row r="105" spans="1:2" customFormat="false">
       <c r="A105" s="0" t="str">
-        <v>53105</v>
+        <v>53106</v>
       </c>
       <c r="B105" s="0" t="str">
-        <v>1005395</v>
+        <v>1005396</v>
       </c>
     </row>
     <row r="106" spans="1:2" customFormat="false">
       <c r="A106" s="0" t="str">
-        <v>53106</v>
+        <v>53107</v>
       </c>
       <c r="B106" s="0" t="str">
-        <v>1005396</v>
+        <v>1005397</v>
       </c>
     </row>
     <row r="107" spans="1:2" customFormat="false">
       <c r="A107" s="0" t="str">
-        <v>53107</v>
+        <v>53108</v>
       </c>
       <c r="B107" s="0" t="str">
-        <v>1005397</v>
+        <v>1005398</v>
       </c>
     </row>
     <row r="108" spans="1:2" customFormat="false">
       <c r="A108" s="0" t="str">
-        <v>53108</v>
+        <v>53109</v>
       </c>
       <c r="B108" s="0" t="str">
-        <v>1005398</v>
+        <v>1005399</v>
       </c>
     </row>
     <row r="109" spans="1:2" customFormat="false">
       <c r="A109" s="0" t="str">
-        <v>53109</v>
+        <v>53110</v>
       </c>
       <c r="B109" s="0" t="str">
-        <v>1005399</v>
+        <v>1005400</v>
       </c>
     </row>
     <row r="110" spans="1:2" customFormat="false">
       <c r="A110" s="0" t="str">
-        <v>53110</v>
+        <v>53111</v>
       </c>
       <c r="B110" s="0" t="str">
-        <v>1005400</v>
+        <v>1005401</v>
       </c>
     </row>
     <row r="111" spans="1:2" customFormat="false">
       <c r="A111" s="0" t="str">
-        <v>53111</v>
+        <v>53112</v>
       </c>
       <c r="B111" s="0" t="str">
-        <v>1005401</v>
+        <v>1005402</v>
       </c>
     </row>
     <row r="112" spans="1:2" customFormat="false">
       <c r="A112" s="0" t="str">
-        <v>53112</v>
+        <v>53113</v>
       </c>
       <c r="B112" s="0" t="str">
-        <v>1005402</v>
+        <v>1005403</v>
       </c>
     </row>
     <row r="113" spans="1:2" customFormat="false">
       <c r="A113" s="0" t="str">
-        <v>53113</v>
+        <v>53114</v>
       </c>
       <c r="B113" s="0" t="str">
-        <v>1005403</v>
+        <v>1005404</v>
       </c>
     </row>
     <row r="114" spans="1:2" customFormat="false">
       <c r="A114" s="0" t="str">
-        <v>53114</v>
+        <v>53115</v>
       </c>
       <c r="B114" s="0" t="str">
-        <v>1005404</v>
+        <v>1005405</v>
       </c>
     </row>
     <row r="115" spans="1:2" customFormat="false">
       <c r="A115" s="0" t="str">
-        <v>53115</v>
+        <v>53116</v>
       </c>
       <c r="B115" s="0" t="str">
-        <v>1005405</v>
+        <v>1005406</v>
       </c>
     </row>
     <row r="116" spans="1:2" customFormat="false">
       <c r="A116" s="0" t="str">
-        <v>53116</v>
+        <v>53117</v>
       </c>
       <c r="B116" s="0" t="str">
-        <v>1005406</v>
+        <v>1005407</v>
       </c>
     </row>
     <row r="117" spans="1:2" customFormat="false">
       <c r="A117" s="0" t="str">
-        <v>53117</v>
+        <v>53118</v>
       </c>
       <c r="B117" s="0" t="str">
-        <v>1005407</v>
+        <v>1005408</v>
       </c>
     </row>
     <row r="118" spans="1:2" customFormat="false">
       <c r="A118" s="0" t="str">
-        <v>53118</v>
+        <v>53119</v>
       </c>
       <c r="B118" s="0" t="str">
-        <v>1005408</v>
+        <v>1005409</v>
       </c>
     </row>
     <row r="119" spans="1:2" customFormat="false">
       <c r="A119" s="0" t="str">
-        <v>53119</v>
+        <v>53120</v>
       </c>
       <c r="B119" s="0" t="str">
-        <v>1005409</v>
+        <v>1005410</v>
       </c>
     </row>
     <row r="120" spans="1:2" customFormat="false">
       <c r="A120" s="0" t="str">
-        <v>53120</v>
+        <v>53121</v>
       </c>
       <c r="B120" s="0" t="str">
-        <v>1005410</v>
+        <v>1005411</v>
       </c>
     </row>
     <row r="121" spans="1:2" customFormat="false">
       <c r="A121" s="0" t="str">
-        <v>53121</v>
+        <v>53122</v>
       </c>
       <c r="B121" s="0" t="str">
-        <v>1005411</v>
+        <v>1005412</v>
       </c>
     </row>
     <row r="122" spans="1:2" customFormat="false">
       <c r="A122" s="0" t="str">
-        <v>53122</v>
+        <v>53123</v>
       </c>
       <c r="B122" s="0" t="str">
-        <v>1005412</v>
+        <v>1005413</v>
       </c>
     </row>
     <row r="123" spans="1:2" customFormat="false">
       <c r="A123" s="0" t="str">
-        <v>53123</v>
+        <v>53124</v>
       </c>
       <c r="B123" s="0" t="str">
-        <v>1005413</v>
+        <v>1005414</v>
       </c>
     </row>
     <row r="124" spans="1:2" customFormat="false">
       <c r="A124" s="0" t="str">
-        <v>53124</v>
+        <v>53125</v>
       </c>
       <c r="B124" s="0" t="str">
-        <v>1005414</v>
+        <v>1005415</v>
       </c>
     </row>
     <row r="125" spans="1:2" customFormat="false">
       <c r="A125" s="0" t="str">
-        <v>53125</v>
+        <v>53126</v>
       </c>
       <c r="B125" s="0" t="str">
-        <v>1005415</v>
+        <v>1005416</v>
       </c>
     </row>
     <row r="126" spans="1:2" customFormat="false">
       <c r="A126" s="0" t="str">
-        <v>53126</v>
+        <v>53127</v>
       </c>
       <c r="B126" s="0" t="str">
-        <v>1005416</v>
+        <v>1005417</v>
       </c>
     </row>
     <row r="127" spans="1:2" customFormat="false">
       <c r="A127" s="0" t="str">
-        <v>53127</v>
+        <v>53128</v>
       </c>
       <c r="B127" s="0" t="str">
-        <v>1005417</v>
+        <v>1005418</v>
       </c>
     </row>
     <row r="128" spans="1:2" customFormat="false">
       <c r="A128" s="0" t="str">
-        <v>53128</v>
+        <v>53129</v>
       </c>
       <c r="B128" s="0" t="str">
-        <v>1005418</v>
+        <v>1005419</v>
       </c>
     </row>
     <row r="129" spans="1:2" customFormat="false">
       <c r="A129" s="0" t="str">
-        <v>53129</v>
+        <v>53130</v>
       </c>
       <c r="B129" s="0" t="str">
-        <v>1005419</v>
+        <v>1005420</v>
       </c>
     </row>
     <row r="130" spans="1:2" customFormat="false">
       <c r="A130" s="0" t="str">
-        <v>53130</v>
+        <v>53131</v>
       </c>
       <c r="B130" s="0" t="str">
-        <v>1005420</v>
+        <v>1005421</v>
       </c>
     </row>
     <row r="131" spans="1:2" customFormat="false">
       <c r="A131" s="0" t="str">
-        <v>53131</v>
+        <v>53132</v>
       </c>
       <c r="B131" s="0" t="str">
-        <v>1005421</v>
+        <v>1005422</v>
       </c>
     </row>
     <row r="132" spans="1:2" customFormat="false">
       <c r="A132" s="0" t="str">
-        <v>53132</v>
+        <v>53133</v>
       </c>
       <c r="B132" s="0" t="str">
-        <v>1005422</v>
+        <v>1005423</v>
       </c>
     </row>
     <row r="133" spans="1:2" customFormat="false">
       <c r="A133" s="0" t="str">
-        <v>53133</v>
+        <v>53134</v>
       </c>
       <c r="B133" s="0" t="str">
-        <v>1005423</v>
+        <v>1005424</v>
       </c>
     </row>
     <row r="134" spans="1:2" customFormat="false">
       <c r="A134" s="0" t="str">
-        <v>53134</v>
+        <v>53135</v>
       </c>
       <c r="B134" s="0" t="str">
-        <v>1005424</v>
+        <v>1005425</v>
       </c>
     </row>
     <row r="135" spans="1:2" customFormat="false">
       <c r="A135" s="0" t="str">
-        <v>53135</v>
+        <v>53136</v>
       </c>
       <c r="B135" s="0" t="str">
-        <v>1005425</v>
+        <v>1005426</v>
       </c>
     </row>
     <row r="136" spans="1:2" customFormat="false">
       <c r="A136" s="0" t="str">
-        <v>53136</v>
+        <v>53137</v>
       </c>
       <c r="B136" s="0" t="str">
-        <v>1005426</v>
+        <v>1005427</v>
       </c>
     </row>
     <row r="137" spans="1:2" customFormat="false">
       <c r="A137" s="0" t="str">
-        <v>53137</v>
+        <v>53138</v>
       </c>
       <c r="B137" s="0" t="str">
-        <v>1005427</v>
+        <v>1005428</v>
       </c>
     </row>
     <row r="138" spans="1:2" customFormat="false">
       <c r="A138" s="0" t="str">
-        <v>53138</v>
+        <v>53139</v>
       </c>
       <c r="B138" s="0" t="str">
-        <v>1005428</v>
+        <v>1005429</v>
       </c>
     </row>
     <row r="139" spans="1:2" customFormat="false">
       <c r="A139" s="0" t="str">
-        <v>53139</v>
+        <v>53140</v>
       </c>
       <c r="B139" s="0" t="str">
-        <v>1005429</v>
+        <v>1005430</v>
       </c>
     </row>
     <row r="140" spans="1:2" customFormat="false">
       <c r="A140" s="0" t="str">
-        <v>53140</v>
+        <v>53141</v>
       </c>
       <c r="B140" s="0" t="str">
-        <v>1005430</v>
+        <v>1005431</v>
       </c>
     </row>
     <row r="141" spans="1:2" customFormat="false">
       <c r="A141" s="0" t="str">
-        <v>53141</v>
+        <v>53142</v>
       </c>
       <c r="B141" s="0" t="str">
-        <v>1005431</v>
+        <v>1005432</v>
       </c>
     </row>
     <row r="142" spans="1:2" customFormat="false">
       <c r="A142" s="0" t="str">
-        <v>53142</v>
+        <v>53143</v>
       </c>
       <c r="B142" s="0" t="str">
-        <v>1005432</v>
+        <v>1005433</v>
       </c>
     </row>
     <row r="143" spans="1:2" customFormat="false">
       <c r="A143" s="0" t="str">
-        <v>53143</v>
+        <v>53144</v>
       </c>
       <c r="B143" s="0" t="str">
-        <v>1005433</v>
+        <v>1005434</v>
       </c>
     </row>
     <row r="144" spans="1:2" customFormat="false">
       <c r="A144" s="0" t="str">
-        <v>53144</v>
+        <v>53145</v>
       </c>
       <c r="B144" s="0" t="str">
-        <v>1005434</v>
+        <v>1005435</v>
       </c>
     </row>
     <row r="145" spans="1:2" customFormat="false">
       <c r="A145" s="0" t="str">
-        <v>53145</v>
+        <v>53147</v>
       </c>
       <c r="B145" s="0" t="str">
-        <v>1005435</v>
+        <v>1005436</v>
       </c>
     </row>
     <row r="146" spans="1:2" customFormat="false">
       <c r="A146" s="0" t="str">
-        <v>53147</v>
+        <v>53149</v>
       </c>
       <c r="B146" s="0" t="str">
-        <v>1005436</v>
+        <v>1005437</v>
       </c>
     </row>
     <row r="147" spans="1:2" customFormat="false">
       <c r="A147" s="0" t="str">
-        <v>53149</v>
+        <v>53151</v>
       </c>
       <c r="B147" s="0" t="str">
-        <v>1005437</v>
+        <v>1005438</v>
       </c>
     </row>
     <row r="148" spans="1:2" customFormat="false">
       <c r="A148" s="0" t="str">
-        <v>53151</v>
+        <v>53153</v>
       </c>
       <c r="B148" s="0" t="str">
-        <v>1005438</v>
+        <v>1005439</v>
       </c>
     </row>
     <row r="149" spans="1:2" customFormat="false">
       <c r="A149" s="0" t="str">
-        <v>53153</v>
+        <v>53155</v>
       </c>
       <c r="B149" s="0" t="str">
-        <v>1005439</v>
+        <v>1005440</v>
       </c>
     </row>
     <row r="150" spans="1:2" customFormat="false">
       <c r="A150" s="0" t="str">
-        <v>53155</v>
+        <v>53157</v>
       </c>
       <c r="B150" s="0" t="str">
-        <v>1005440</v>
+        <v>1005441</v>
       </c>
     </row>
     <row r="151" spans="1:2" customFormat="false">
       <c r="A151" s="0" t="str">
-        <v>53157</v>
+        <v>53159</v>
       </c>
       <c r="B151" s="0" t="str">
-        <v>1005441</v>
+        <v>1005442</v>
       </c>
     </row>
     <row r="152" spans="1:2" customFormat="false">
       <c r="A152" s="0" t="str">
-        <v>53159</v>
+        <v>53161</v>
       </c>
       <c r="B152" s="0" t="str">
-        <v>1005442</v>
+        <v>1005443</v>
       </c>
     </row>
     <row r="153" spans="1:2" customFormat="false">
       <c r="A153" s="0" t="str">
-        <v>53161</v>
+        <v>53163</v>
       </c>
       <c r="B153" s="0" t="str">
-        <v>1005443</v>
+        <v>1005444</v>
       </c>
     </row>
     <row r="154" spans="1:2" customFormat="false">
       <c r="A154" s="0" t="str">
-        <v>53163</v>
+        <v>53165</v>
       </c>
       <c r="B154" s="0" t="str">
-        <v>1005444</v>
+        <v>1005445</v>
       </c>
     </row>
     <row r="155" spans="1:2" customFormat="false">
       <c r="A155" s="0" t="str">
-        <v>53165</v>
+        <v>53167</v>
       </c>
       <c r="B155" s="0" t="str">
-        <v>1005445</v>
+        <v>1005446</v>
       </c>
     </row>
     <row r="156" spans="1:2" customFormat="false">
       <c r="A156" s="0" t="str">
-        <v>53167</v>
+        <v>53169</v>
       </c>
       <c r="B156" s="0" t="str">
-        <v>1005446</v>
+        <v>1005447</v>
       </c>
     </row>
     <row r="157" spans="1:2" customFormat="false">
       <c r="A157" s="0" t="str">
-        <v>53169</v>
+        <v>53171</v>
       </c>
       <c r="B157" s="0" t="str">
-        <v>1005447</v>
+        <v>1005448</v>
       </c>
     </row>
     <row r="158" spans="1:2" customFormat="false">
       <c r="A158" s="0" t="str">
-        <v>53171</v>
+        <v>53173</v>
       </c>
       <c r="B158" s="0" t="str">
-        <v>1005448</v>
+        <v>1005449</v>
       </c>
     </row>
     <row r="159" spans="1:2" customFormat="false">
       <c r="A159" s="0" t="str">
-        <v>53173</v>
+        <v>53175</v>
       </c>
       <c r="B159" s="0" t="str">
-        <v>1005449</v>
+        <v>1005450</v>
       </c>
     </row>
     <row r="160" spans="1:2" customFormat="false">
       <c r="A160" s="0" t="str">
-        <v>53175</v>
+        <v>53177</v>
       </c>
       <c r="B160" s="0" t="str">
-        <v>1005450</v>
+        <v>1005451</v>
       </c>
     </row>
     <row r="161" spans="1:2" customFormat="false">
       <c r="A161" s="0" t="str">
-        <v>53177</v>
+        <v>53179</v>
       </c>
       <c r="B161" s="0" t="str">
-        <v>1005451</v>
+        <v>1005452</v>
       </c>
     </row>
     <row r="162" spans="1:2" customFormat="false">
       <c r="A162" s="0" t="str">
-        <v>53179</v>
+        <v>53181</v>
       </c>
       <c r="B162" s="0" t="str">
-        <v>1005452</v>
+        <v>1005453</v>
       </c>
     </row>
     <row r="163" spans="1:2" customFormat="false">
       <c r="A163" s="0" t="str">
-        <v>53181</v>
+        <v>53185</v>
       </c>
       <c r="B163" s="0" t="str">
-        <v>1005453</v>
+        <v>1005455</v>
       </c>
     </row>
     <row r="164" spans="1:2" customFormat="false">
       <c r="A164" s="0" t="str">
-        <v>53185</v>
+        <v>53187</v>
       </c>
       <c r="B164" s="0" t="str">
-        <v>1005455</v>
+        <v>1005456</v>
       </c>
     </row>
     <row r="165" spans="1:2" customFormat="false">
       <c r="A165" s="0" t="str">
-        <v>53187</v>
+        <v>53189</v>
       </c>
       <c r="B165" s="0" t="str">
-        <v>1005456</v>
+        <v>1005457</v>
       </c>
     </row>
     <row r="166" spans="1:2" customFormat="false">
       <c r="A166" s="0" t="str">
-        <v>53189</v>
+        <v>53191</v>
       </c>
       <c r="B166" s="0" t="str">
-        <v>1005457</v>
+        <v>1005458</v>
       </c>
     </row>
     <row r="167" spans="1:2" customFormat="false">
       <c r="A167" s="0" t="str">
-        <v>53191</v>
+        <v>53183</v>
       </c>
       <c r="B167" s="0" t="str">
-        <v>1005458</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" customFormat="false">
-      <c r="A168" s="0" t="str">
-        <v>53183</v>
-      </c>
-      <c r="B168" s="0" t="str">
         <v>1005454</v>
       </c>
     </row>
@@ -38754,122 +38746,122 @@
     </row>
     <row r="80" spans="1:2" customFormat="false">
       <c r="A80" s="0" t="str">
-        <v>73080</v>
+        <v>73081</v>
       </c>
       <c r="B80" s="0" t="str">
-        <v>1005790</v>
+        <v>1005791</v>
       </c>
     </row>
     <row r="81" spans="1:2" customFormat="false">
       <c r="A81" s="0" t="str">
-        <v>73081</v>
+        <v>73082</v>
       </c>
       <c r="B81" s="0" t="str">
-        <v>1005791</v>
+        <v>1005792</v>
       </c>
     </row>
     <row r="82" spans="1:2" customFormat="false">
       <c r="A82" s="0" t="str">
-        <v>73082</v>
+        <v>73083</v>
       </c>
       <c r="B82" s="0" t="str">
-        <v>1005792</v>
+        <v>1005793</v>
       </c>
     </row>
     <row r="83" spans="1:2" customFormat="false">
       <c r="A83" s="0" t="str">
-        <v>73083</v>
+        <v>73084</v>
       </c>
       <c r="B83" s="0" t="str">
-        <v>1005793</v>
+        <v>1005794</v>
       </c>
     </row>
     <row r="84" spans="1:2" customFormat="false">
       <c r="A84" s="0" t="str">
-        <v>73084</v>
+        <v>73085</v>
       </c>
       <c r="B84" s="0" t="str">
-        <v>1005794</v>
+        <v>1005795</v>
       </c>
     </row>
     <row r="85" spans="1:2" customFormat="false">
       <c r="A85" s="0" t="str">
-        <v>73085</v>
+        <v>73086</v>
       </c>
       <c r="B85" s="0" t="str">
-        <v>1005795</v>
+        <v>1005796</v>
       </c>
     </row>
     <row r="86" spans="1:2" customFormat="false">
       <c r="A86" s="0" t="str">
-        <v>73086</v>
+        <v>73087</v>
       </c>
       <c r="B86" s="0" t="str">
-        <v>1005796</v>
+        <v>1005797</v>
       </c>
     </row>
     <row r="87" spans="1:2" customFormat="false">
       <c r="A87" s="0" t="str">
-        <v>73087</v>
+        <v>73088</v>
       </c>
       <c r="B87" s="0" t="str">
-        <v>1005797</v>
+        <v>1005798</v>
       </c>
     </row>
     <row r="88" spans="1:2" customFormat="false">
       <c r="A88" s="0" t="str">
-        <v>73088</v>
+        <v>73089</v>
       </c>
       <c r="B88" s="0" t="str">
-        <v>1005798</v>
+        <v>1005799</v>
       </c>
     </row>
     <row r="89" spans="1:2" customFormat="false">
       <c r="A89" s="0" t="str">
-        <v>73089</v>
+        <v>73090</v>
       </c>
       <c r="B89" s="0" t="str">
-        <v>1005799</v>
+        <v>1005800</v>
       </c>
     </row>
     <row r="90" spans="1:2" customFormat="false">
       <c r="A90" s="0" t="str">
-        <v>73090</v>
+        <v>73091</v>
       </c>
       <c r="B90" s="0" t="str">
-        <v>1005800</v>
+        <v>1005801</v>
       </c>
     </row>
     <row r="91" spans="1:2" customFormat="false">
       <c r="A91" s="0" t="str">
-        <v>73091</v>
+        <v>73092</v>
       </c>
       <c r="B91" s="0" t="str">
-        <v>1005801</v>
+        <v>1005802</v>
       </c>
     </row>
     <row r="92" spans="1:2" customFormat="false">
       <c r="A92" s="0" t="str">
-        <v>73092</v>
+        <v>73093</v>
       </c>
       <c r="B92" s="0" t="str">
-        <v>1005802</v>
+        <v>1005803</v>
       </c>
     </row>
     <row r="93" spans="1:2" customFormat="false">
       <c r="A93" s="0" t="str">
-        <v>73093</v>
+        <v>73094</v>
       </c>
       <c r="B93" s="0" t="str">
-        <v>1005803</v>
+        <v>1005804</v>
       </c>
     </row>
     <row r="94" spans="1:2" customFormat="false">
       <c r="A94" s="0" t="str">
-        <v>73094</v>
+        <v>73080</v>
       </c>
       <c r="B94" s="0" t="str">
-        <v>1005804</v>
+        <v>1005790</v>
       </c>
     </row>
   </sheetData>
@@ -38878,7 +38870,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetData>
     <row r="1" spans="1:2" customFormat="false">
       <c r="A1" s="0" t="str">
@@ -38886,6 +38878,22 @@
       </c>
       <c r="B1" s="0" t="str">
         <v>Lockeruniq</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" customFormat="false">
+      <c r="A2" s="0" t="str">
+        <v>406527</v>
+      </c>
+      <c r="B2" s="0" t="str">
+        <v>1005315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" customFormat="false">
+      <c r="A3" s="0" t="str">
+        <v>304532</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <v>1005315</v>
       </c>
     </row>
   </sheetData>
@@ -39238,7 +39246,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <dimension ref="A1:B222"/>
+  <dimension ref="A1:B228"/>
   <sheetData>
     <row r="1" spans="1:2" customFormat="false">
       <c r="A1" s="0" t="str">
@@ -41014,6 +41022,54 @@
       </c>
       <c r="B222" s="0" t="str">
         <v>1004221</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" customFormat="false">
+      <c r="A223" s="0" t="str">
+        <v>6010</v>
+      </c>
+      <c r="B223" s="0" t="str">
+        <v>1004121</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" customFormat="false">
+      <c r="A224" s="0" t="str">
+        <v>6045</v>
+      </c>
+      <c r="B224" s="0" t="str">
+        <v>1004155</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" customFormat="false">
+      <c r="A225" s="0" t="str">
+        <v>6004</v>
+      </c>
+      <c r="B225" s="0" t="str">
+        <v>1004115</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" customFormat="false">
+      <c r="A226" s="0" t="str">
+        <v>5164</v>
+      </c>
+      <c r="B226" s="0" t="str">
+        <v>1004104</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" customFormat="false">
+      <c r="A227" s="0" t="str">
+        <v>5154</v>
+      </c>
+      <c r="B227" s="0" t="str">
+        <v>1004094</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" customFormat="false">
+      <c r="A228" s="0" t="str">
+        <v>5169</v>
+      </c>
+      <c r="B228" s="0" t="str">
+        <v>1004109</v>
       </c>
     </row>
   </sheetData>
@@ -41022,7 +41078,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <dimension ref="A1:B224"/>
+  <dimension ref="A1:B217"/>
   <sheetData>
     <row r="1" spans="1:2" customFormat="false">
       <c r="A1" s="0" t="str">
@@ -41386,1433 +41442,1377 @@
     </row>
     <row r="46" spans="1:2" customFormat="false">
       <c r="A46" s="0" t="str">
-        <v>5154</v>
+        <v>5155</v>
       </c>
       <c r="B46" s="0" t="str">
-        <v>1004094</v>
+        <v>1004095</v>
       </c>
     </row>
     <row r="47" spans="1:2" customFormat="false">
       <c r="A47" s="0" t="str">
-        <v>5155</v>
+        <v>5156</v>
       </c>
       <c r="B47" s="0" t="str">
-        <v>1004095</v>
+        <v>1004096</v>
       </c>
     </row>
     <row r="48" spans="1:2" customFormat="false">
       <c r="A48" s="0" t="str">
-        <v>5156</v>
+        <v>5157</v>
       </c>
       <c r="B48" s="0" t="str">
-        <v>1004096</v>
+        <v>1004097</v>
       </c>
     </row>
     <row r="49" spans="1:2" customFormat="false">
       <c r="A49" s="0" t="str">
-        <v>5157</v>
+        <v>5158</v>
       </c>
       <c r="B49" s="0" t="str">
-        <v>1004097</v>
+        <v>1004098</v>
       </c>
     </row>
     <row r="50" spans="1:2" customFormat="false">
       <c r="A50" s="0" t="str">
-        <v>5158</v>
+        <v>5159</v>
       </c>
       <c r="B50" s="0" t="str">
-        <v>1004098</v>
+        <v>1004099</v>
       </c>
     </row>
     <row r="51" spans="1:2" customFormat="false">
       <c r="A51" s="0" t="str">
-        <v>5159</v>
+        <v>5160</v>
       </c>
       <c r="B51" s="0" t="str">
-        <v>1004099</v>
+        <v>1004100</v>
       </c>
     </row>
     <row r="52" spans="1:2" customFormat="false">
       <c r="A52" s="0" t="str">
-        <v>5160</v>
+        <v>5161</v>
       </c>
       <c r="B52" s="0" t="str">
-        <v>1004100</v>
+        <v>1004101</v>
       </c>
     </row>
     <row r="53" spans="1:2" customFormat="false">
       <c r="A53" s="0" t="str">
-        <v>5161</v>
+        <v>5162</v>
       </c>
       <c r="B53" s="0" t="str">
-        <v>1004101</v>
+        <v>1004102</v>
       </c>
     </row>
     <row r="54" spans="1:2" customFormat="false">
       <c r="A54" s="0" t="str">
-        <v>5162</v>
+        <v>5163</v>
       </c>
       <c r="B54" s="0" t="str">
-        <v>1004102</v>
+        <v>1004103</v>
       </c>
     </row>
     <row r="55" spans="1:2" customFormat="false">
       <c r="A55" s="0" t="str">
-        <v>5163</v>
+        <v>5165</v>
       </c>
       <c r="B55" s="0" t="str">
-        <v>1004103</v>
+        <v>1004105</v>
       </c>
     </row>
     <row r="56" spans="1:2" customFormat="false">
       <c r="A56" s="0" t="str">
-        <v>5164</v>
+        <v>5166</v>
       </c>
       <c r="B56" s="0" t="str">
-        <v>1004104</v>
+        <v>1004106</v>
       </c>
     </row>
     <row r="57" spans="1:2" customFormat="false">
       <c r="A57" s="0" t="str">
-        <v>5165</v>
+        <v>5167</v>
       </c>
       <c r="B57" s="0" t="str">
-        <v>1004105</v>
+        <v>1004107</v>
       </c>
     </row>
     <row r="58" spans="1:2" customFormat="false">
       <c r="A58" s="0" t="str">
-        <v>5166</v>
+        <v>5168</v>
       </c>
       <c r="B58" s="0" t="str">
-        <v>1004106</v>
+        <v>1004108</v>
       </c>
     </row>
     <row r="59" spans="1:2" customFormat="false">
       <c r="A59" s="0" t="str">
-        <v>5167</v>
+        <v>5170</v>
       </c>
       <c r="B59" s="0" t="str">
-        <v>1004107</v>
+        <v>1004110</v>
       </c>
     </row>
     <row r="60" spans="1:2" customFormat="false">
       <c r="A60" s="0" t="str">
-        <v>5168</v>
+        <v>6000</v>
       </c>
       <c r="B60" s="0" t="str">
-        <v>1004108</v>
+        <v>1004111</v>
       </c>
     </row>
     <row r="61" spans="1:2" customFormat="false">
       <c r="A61" s="0" t="str">
-        <v>5169</v>
+        <v>6001</v>
       </c>
       <c r="B61" s="0" t="str">
-        <v>1004109</v>
+        <v>1004112</v>
       </c>
     </row>
     <row r="62" spans="1:2" customFormat="false">
       <c r="A62" s="0" t="str">
-        <v>5170</v>
+        <v>6002</v>
       </c>
       <c r="B62" s="0" t="str">
-        <v>1004110</v>
+        <v>1004113</v>
       </c>
     </row>
     <row r="63" spans="1:2" customFormat="false">
       <c r="A63" s="0" t="str">
-        <v>6000</v>
+        <v>6003</v>
       </c>
       <c r="B63" s="0" t="str">
-        <v>1004111</v>
+        <v>1004114</v>
       </c>
     </row>
     <row r="64" spans="1:2" customFormat="false">
       <c r="A64" s="0" t="str">
-        <v>6001</v>
+        <v>6005</v>
       </c>
       <c r="B64" s="0" t="str">
-        <v>1004112</v>
+        <v>1004116</v>
       </c>
     </row>
     <row r="65" spans="1:2" customFormat="false">
       <c r="A65" s="0" t="str">
-        <v>6002</v>
+        <v>6006</v>
       </c>
       <c r="B65" s="0" t="str">
-        <v>1004113</v>
+        <v>1004117</v>
       </c>
     </row>
     <row r="66" spans="1:2" customFormat="false">
       <c r="A66" s="0" t="str">
-        <v>6003</v>
+        <v>6007</v>
       </c>
       <c r="B66" s="0" t="str">
-        <v>1004114</v>
+        <v>1004118</v>
       </c>
     </row>
     <row r="67" spans="1:2" customFormat="false">
       <c r="A67" s="0" t="str">
-        <v>6004</v>
+        <v>6008</v>
       </c>
       <c r="B67" s="0" t="str">
-        <v>1004115</v>
+        <v>1004119</v>
       </c>
     </row>
     <row r="68" spans="1:2" customFormat="false">
       <c r="A68" s="0" t="str">
-        <v>6005</v>
+        <v>6009</v>
       </c>
       <c r="B68" s="0" t="str">
-        <v>1004116</v>
+        <v>1004120</v>
       </c>
     </row>
     <row r="69" spans="1:2" customFormat="false">
       <c r="A69" s="0" t="str">
-        <v>6006</v>
+        <v>6011</v>
       </c>
       <c r="B69" s="0" t="str">
-        <v>1004117</v>
+        <v>1004122</v>
       </c>
     </row>
     <row r="70" spans="1:2" customFormat="false">
       <c r="A70" s="0" t="str">
-        <v>6007</v>
+        <v>6012</v>
       </c>
       <c r="B70" s="0" t="str">
-        <v>1004118</v>
+        <v>1004123</v>
       </c>
     </row>
     <row r="71" spans="1:2" customFormat="false">
       <c r="A71" s="0" t="str">
-        <v>6008</v>
+        <v>6013</v>
       </c>
       <c r="B71" s="0" t="str">
-        <v>1004119</v>
+        <v>1004124</v>
       </c>
     </row>
     <row r="72" spans="1:2" customFormat="false">
       <c r="A72" s="0" t="str">
-        <v>6009</v>
+        <v>6014</v>
       </c>
       <c r="B72" s="0" t="str">
-        <v>1004120</v>
+        <v>1004125</v>
       </c>
     </row>
     <row r="73" spans="1:2" customFormat="false">
       <c r="A73" s="0" t="str">
-        <v>6010</v>
+        <v>6015</v>
       </c>
       <c r="B73" s="0" t="str">
-        <v>1004121</v>
+        <v>1004126</v>
       </c>
     </row>
     <row r="74" spans="1:2" customFormat="false">
       <c r="A74" s="0" t="str">
-        <v>6011</v>
+        <v>6016</v>
       </c>
       <c r="B74" s="0" t="str">
-        <v>1004122</v>
+        <v>1004127</v>
       </c>
     </row>
     <row r="75" spans="1:2" customFormat="false">
       <c r="A75" s="0" t="str">
-        <v>6012</v>
+        <v>6017</v>
       </c>
       <c r="B75" s="0" t="str">
-        <v>1004123</v>
+        <v>1004128</v>
       </c>
     </row>
     <row r="76" spans="1:2" customFormat="false">
       <c r="A76" s="0" t="str">
-        <v>6013</v>
+        <v>6018</v>
       </c>
       <c r="B76" s="0" t="str">
-        <v>1004124</v>
+        <v>1004129</v>
       </c>
     </row>
     <row r="77" spans="1:2" customFormat="false">
       <c r="A77" s="0" t="str">
-        <v>6014</v>
+        <v>6019</v>
       </c>
       <c r="B77" s="0" t="str">
-        <v>1004125</v>
+        <v>1004130</v>
       </c>
     </row>
     <row r="78" spans="1:2" customFormat="false">
       <c r="A78" s="0" t="str">
-        <v>6015</v>
+        <v>6020</v>
       </c>
       <c r="B78" s="0" t="str">
-        <v>1004126</v>
+        <v>1004131</v>
       </c>
     </row>
     <row r="79" spans="1:2" customFormat="false">
       <c r="A79" s="0" t="str">
-        <v>6016</v>
+        <v>6021</v>
       </c>
       <c r="B79" s="0" t="str">
-        <v>1004127</v>
+        <v>1004132</v>
       </c>
     </row>
     <row r="80" spans="1:2" customFormat="false">
       <c r="A80" s="0" t="str">
-        <v>6017</v>
+        <v>6023</v>
       </c>
       <c r="B80" s="0" t="str">
-        <v>1004128</v>
+        <v>1004133</v>
       </c>
     </row>
     <row r="81" spans="1:2" customFormat="false">
       <c r="A81" s="0" t="str">
-        <v>6018</v>
+        <v>6024</v>
       </c>
       <c r="B81" s="0" t="str">
-        <v>1004129</v>
+        <v>1004134</v>
       </c>
     </row>
     <row r="82" spans="1:2" customFormat="false">
       <c r="A82" s="0" t="str">
-        <v>6019</v>
+        <v>6025</v>
       </c>
       <c r="B82" s="0" t="str">
-        <v>1004130</v>
+        <v>1004135</v>
       </c>
     </row>
     <row r="83" spans="1:2" customFormat="false">
       <c r="A83" s="0" t="str">
-        <v>6020</v>
+        <v>6026</v>
       </c>
       <c r="B83" s="0" t="str">
-        <v>1004131</v>
+        <v>1004136</v>
       </c>
     </row>
     <row r="84" spans="1:2" customFormat="false">
       <c r="A84" s="0" t="str">
-        <v>6021</v>
+        <v>6027</v>
       </c>
       <c r="B84" s="0" t="str">
-        <v>1004132</v>
+        <v>1004137</v>
       </c>
     </row>
     <row r="85" spans="1:2" customFormat="false">
       <c r="A85" s="0" t="str">
-        <v>6023</v>
+        <v>6028</v>
       </c>
       <c r="B85" s="0" t="str">
-        <v>1004133</v>
+        <v>1004138</v>
       </c>
     </row>
     <row r="86" spans="1:2" customFormat="false">
       <c r="A86" s="0" t="str">
-        <v>6024</v>
+        <v>6029</v>
       </c>
       <c r="B86" s="0" t="str">
-        <v>1004134</v>
+        <v>1004139</v>
       </c>
     </row>
     <row r="87" spans="1:2" customFormat="false">
       <c r="A87" s="0" t="str">
-        <v>6025</v>
+        <v>6030</v>
       </c>
       <c r="B87" s="0" t="str">
-        <v>1004135</v>
+        <v>1004140</v>
       </c>
     </row>
     <row r="88" spans="1:2" customFormat="false">
       <c r="A88" s="0" t="str">
-        <v>6026</v>
+        <v>6031</v>
       </c>
       <c r="B88" s="0" t="str">
-        <v>1004136</v>
+        <v>1004141</v>
       </c>
     </row>
     <row r="89" spans="1:2" customFormat="false">
       <c r="A89" s="0" t="str">
-        <v>6027</v>
+        <v>6032</v>
       </c>
       <c r="B89" s="0" t="str">
-        <v>1004137</v>
+        <v>1004142</v>
       </c>
     </row>
     <row r="90" spans="1:2" customFormat="false">
       <c r="A90" s="0" t="str">
-        <v>6028</v>
+        <v>6033</v>
       </c>
       <c r="B90" s="0" t="str">
-        <v>1004138</v>
+        <v>1004143</v>
       </c>
     </row>
     <row r="91" spans="1:2" customFormat="false">
       <c r="A91" s="0" t="str">
-        <v>6029</v>
+        <v>6034</v>
       </c>
       <c r="B91" s="0" t="str">
-        <v>1004139</v>
+        <v>1004144</v>
       </c>
     </row>
     <row r="92" spans="1:2" customFormat="false">
       <c r="A92" s="0" t="str">
-        <v>6030</v>
+        <v>6035</v>
       </c>
       <c r="B92" s="0" t="str">
-        <v>1004140</v>
+        <v>1004145</v>
       </c>
     </row>
     <row r="93" spans="1:2" customFormat="false">
       <c r="A93" s="0" t="str">
-        <v>6031</v>
+        <v>6036</v>
       </c>
       <c r="B93" s="0" t="str">
-        <v>1004141</v>
+        <v>1004146</v>
       </c>
     </row>
     <row r="94" spans="1:2" customFormat="false">
       <c r="A94" s="0" t="str">
-        <v>6032</v>
+        <v>6037</v>
       </c>
       <c r="B94" s="0" t="str">
-        <v>1004142</v>
+        <v>1004147</v>
       </c>
     </row>
     <row r="95" spans="1:2" customFormat="false">
       <c r="A95" s="0" t="str">
-        <v>6033</v>
+        <v>6038</v>
       </c>
       <c r="B95" s="0" t="str">
-        <v>1004143</v>
+        <v>1004148</v>
       </c>
     </row>
     <row r="96" spans="1:2" customFormat="false">
       <c r="A96" s="0" t="str">
-        <v>6034</v>
+        <v>6039</v>
       </c>
       <c r="B96" s="0" t="str">
-        <v>1004144</v>
+        <v>1004149</v>
       </c>
     </row>
     <row r="97" spans="1:2" customFormat="false">
       <c r="A97" s="0" t="str">
-        <v>6035</v>
+        <v>6040</v>
       </c>
       <c r="B97" s="0" t="str">
-        <v>1004145</v>
+        <v>1004150</v>
       </c>
     </row>
     <row r="98" spans="1:2" customFormat="false">
       <c r="A98" s="0" t="str">
-        <v>6036</v>
+        <v>6041</v>
       </c>
       <c r="B98" s="0" t="str">
-        <v>1004146</v>
+        <v>1004151</v>
       </c>
     </row>
     <row r="99" spans="1:2" customFormat="false">
       <c r="A99" s="0" t="str">
-        <v>6037</v>
+        <v>6042</v>
       </c>
       <c r="B99" s="0" t="str">
-        <v>1004147</v>
+        <v>1004152</v>
       </c>
     </row>
     <row r="100" spans="1:2" customFormat="false">
       <c r="A100" s="0" t="str">
-        <v>6038</v>
+        <v>6043</v>
       </c>
       <c r="B100" s="0" t="str">
-        <v>1004148</v>
+        <v>1004153</v>
       </c>
     </row>
     <row r="101" spans="1:2" customFormat="false">
       <c r="A101" s="0" t="str">
-        <v>6039</v>
+        <v>6044</v>
       </c>
       <c r="B101" s="0" t="str">
-        <v>1004149</v>
+        <v>1004154</v>
       </c>
     </row>
     <row r="102" spans="1:2" customFormat="false">
       <c r="A102" s="0" t="str">
-        <v>6040</v>
+        <v>6046</v>
       </c>
       <c r="B102" s="0" t="str">
-        <v>1004150</v>
+        <v>1004156</v>
       </c>
     </row>
     <row r="103" spans="1:2" customFormat="false">
       <c r="A103" s="0" t="str">
-        <v>6041</v>
+        <v>6047</v>
       </c>
       <c r="B103" s="0" t="str">
-        <v>1004151</v>
+        <v>1004157</v>
       </c>
     </row>
     <row r="104" spans="1:2" customFormat="false">
       <c r="A104" s="0" t="str">
-        <v>6042</v>
+        <v>6048</v>
       </c>
       <c r="B104" s="0" t="str">
-        <v>1004152</v>
+        <v>1004158</v>
       </c>
     </row>
     <row r="105" spans="1:2" customFormat="false">
       <c r="A105" s="0" t="str">
-        <v>6043</v>
+        <v>6049</v>
       </c>
       <c r="B105" s="0" t="str">
-        <v>1004153</v>
+        <v>1004159</v>
       </c>
     </row>
     <row r="106" spans="1:2" customFormat="false">
       <c r="A106" s="0" t="str">
-        <v>6044</v>
+        <v>6050</v>
       </c>
       <c r="B106" s="0" t="str">
-        <v>1004154</v>
+        <v>1004160</v>
       </c>
     </row>
     <row r="107" spans="1:2" customFormat="false">
       <c r="A107" s="0" t="str">
-        <v>6045</v>
+        <v>6051</v>
       </c>
       <c r="B107" s="0" t="str">
-        <v>1004155</v>
+        <v>1004161</v>
       </c>
     </row>
     <row r="108" spans="1:2" customFormat="false">
       <c r="A108" s="0" t="str">
-        <v>6046</v>
+        <v>6052</v>
       </c>
       <c r="B108" s="0" t="str">
-        <v>1004156</v>
+        <v>1004162</v>
       </c>
     </row>
     <row r="109" spans="1:2" customFormat="false">
       <c r="A109" s="0" t="str">
-        <v>6047</v>
+        <v>6053</v>
       </c>
       <c r="B109" s="0" t="str">
-        <v>1004157</v>
+        <v>1004163</v>
       </c>
     </row>
     <row r="110" spans="1:2" customFormat="false">
       <c r="A110" s="0" t="str">
-        <v>6048</v>
+        <v>6054</v>
       </c>
       <c r="B110" s="0" t="str">
-        <v>1004158</v>
+        <v>1004164</v>
       </c>
     </row>
     <row r="111" spans="1:2" customFormat="false">
       <c r="A111" s="0" t="str">
-        <v>6049</v>
+        <v>6055</v>
       </c>
       <c r="B111" s="0" t="str">
-        <v>1004159</v>
+        <v>1004165</v>
       </c>
     </row>
     <row r="112" spans="1:2" customFormat="false">
       <c r="A112" s="0" t="str">
-        <v>6050</v>
+        <v>6056</v>
       </c>
       <c r="B112" s="0" t="str">
-        <v>1004160</v>
+        <v>1004166</v>
       </c>
     </row>
     <row r="113" spans="1:2" customFormat="false">
       <c r="A113" s="0" t="str">
-        <v>6051</v>
+        <v>6057</v>
       </c>
       <c r="B113" s="0" t="str">
-        <v>1004161</v>
+        <v>1004167</v>
       </c>
     </row>
     <row r="114" spans="1:2" customFormat="false">
       <c r="A114" s="0" t="str">
-        <v>6052</v>
+        <v>6058</v>
       </c>
       <c r="B114" s="0" t="str">
-        <v>1004162</v>
+        <v>1004168</v>
       </c>
     </row>
     <row r="115" spans="1:2" customFormat="false">
       <c r="A115" s="0" t="str">
-        <v>6053</v>
+        <v>6060</v>
       </c>
       <c r="B115" s="0" t="str">
-        <v>1004163</v>
+        <v>1004169</v>
       </c>
     </row>
     <row r="116" spans="1:2" customFormat="false">
       <c r="A116" s="0" t="str">
-        <v>6054</v>
+        <v>6061</v>
       </c>
       <c r="B116" s="0" t="str">
-        <v>1004164</v>
+        <v>1004170</v>
       </c>
     </row>
     <row r="117" spans="1:2" customFormat="false">
       <c r="A117" s="0" t="str">
-        <v>6055</v>
+        <v>6062</v>
       </c>
       <c r="B117" s="0" t="str">
-        <v>1004165</v>
+        <v>1004171</v>
       </c>
     </row>
     <row r="118" spans="1:2" customFormat="false">
       <c r="A118" s="0" t="str">
-        <v>6056</v>
+        <v>6063</v>
       </c>
       <c r="B118" s="0" t="str">
-        <v>1004166</v>
+        <v>1004172</v>
       </c>
     </row>
     <row r="119" spans="1:2" customFormat="false">
       <c r="A119" s="0" t="str">
-        <v>6057</v>
+        <v>6064</v>
       </c>
       <c r="B119" s="0" t="str">
-        <v>1004167</v>
+        <v>1004173</v>
       </c>
     </row>
     <row r="120" spans="1:2" customFormat="false">
       <c r="A120" s="0" t="str">
-        <v>6058</v>
+        <v>6065</v>
       </c>
       <c r="B120" s="0" t="str">
-        <v>1004168</v>
+        <v>1004174</v>
       </c>
     </row>
     <row r="121" spans="1:2" customFormat="false">
       <c r="A121" s="0" t="str">
-        <v>6060</v>
+        <v>6066</v>
       </c>
       <c r="B121" s="0" t="str">
-        <v>1004169</v>
+        <v>1004175</v>
       </c>
     </row>
     <row r="122" spans="1:2" customFormat="false">
       <c r="A122" s="0" t="str">
-        <v>6061</v>
+        <v>6067</v>
       </c>
       <c r="B122" s="0" t="str">
-        <v>1004170</v>
+        <v>1004176</v>
       </c>
     </row>
     <row r="123" spans="1:2" customFormat="false">
       <c r="A123" s="0" t="str">
-        <v>6062</v>
+        <v>6068</v>
       </c>
       <c r="B123" s="0" t="str">
-        <v>1004171</v>
+        <v>1004177</v>
       </c>
     </row>
     <row r="124" spans="1:2" customFormat="false">
       <c r="A124" s="0" t="str">
-        <v>6063</v>
+        <v>6069</v>
       </c>
       <c r="B124" s="0" t="str">
-        <v>1004172</v>
+        <v>1004178</v>
       </c>
     </row>
     <row r="125" spans="1:2" customFormat="false">
       <c r="A125" s="0" t="str">
-        <v>6064</v>
+        <v>6070</v>
       </c>
       <c r="B125" s="0" t="str">
-        <v>1004173</v>
+        <v>1004179</v>
       </c>
     </row>
     <row r="126" spans="1:2" customFormat="false">
       <c r="A126" s="0" t="str">
-        <v>6065</v>
+        <v>6071</v>
       </c>
       <c r="B126" s="0" t="str">
-        <v>1004174</v>
+        <v>1004180</v>
       </c>
     </row>
     <row r="127" spans="1:2" customFormat="false">
       <c r="A127" s="0" t="str">
-        <v>6066</v>
+        <v>6072</v>
       </c>
       <c r="B127" s="0" t="str">
-        <v>1004175</v>
+        <v>1004181</v>
       </c>
     </row>
     <row r="128" spans="1:2" customFormat="false">
       <c r="A128" s="0" t="str">
-        <v>6067</v>
+        <v>6073</v>
       </c>
       <c r="B128" s="0" t="str">
-        <v>1004176</v>
+        <v>1004182</v>
       </c>
     </row>
     <row r="129" spans="1:2" customFormat="false">
       <c r="A129" s="0" t="str">
-        <v>6068</v>
+        <v>6074</v>
       </c>
       <c r="B129" s="0" t="str">
-        <v>1004177</v>
+        <v>1004183</v>
       </c>
     </row>
     <row r="130" spans="1:2" customFormat="false">
       <c r="A130" s="0" t="str">
-        <v>6069</v>
+        <v>6075</v>
       </c>
       <c r="B130" s="0" t="str">
-        <v>1004178</v>
+        <v>1004184</v>
       </c>
     </row>
     <row r="131" spans="1:2" customFormat="false">
       <c r="A131" s="0" t="str">
-        <v>6070</v>
+        <v>6076</v>
       </c>
       <c r="B131" s="0" t="str">
-        <v>1004179</v>
+        <v>1004185</v>
       </c>
     </row>
     <row r="132" spans="1:2" customFormat="false">
       <c r="A132" s="0" t="str">
-        <v>6071</v>
+        <v>6077</v>
       </c>
       <c r="B132" s="0" t="str">
-        <v>1004180</v>
+        <v>1004186</v>
       </c>
     </row>
     <row r="133" spans="1:2" customFormat="false">
       <c r="A133" s="0" t="str">
-        <v>6072</v>
+        <v>6078</v>
       </c>
       <c r="B133" s="0" t="str">
-        <v>1004181</v>
+        <v>1004187</v>
       </c>
     </row>
     <row r="134" spans="1:2" customFormat="false">
       <c r="A134" s="0" t="str">
-        <v>6073</v>
+        <v>6080</v>
       </c>
       <c r="B134" s="0" t="str">
-        <v>1004182</v>
+        <v>1004189</v>
       </c>
     </row>
     <row r="135" spans="1:2" customFormat="false">
       <c r="A135" s="0" t="str">
-        <v>6074</v>
+        <v>6081</v>
       </c>
       <c r="B135" s="0" t="str">
-        <v>1004183</v>
+        <v>1004190</v>
       </c>
     </row>
     <row r="136" spans="1:2" customFormat="false">
       <c r="A136" s="0" t="str">
-        <v>6075</v>
+        <v>6082</v>
       </c>
       <c r="B136" s="0" t="str">
-        <v>1004184</v>
+        <v>1004191</v>
       </c>
     </row>
     <row r="137" spans="1:2" customFormat="false">
       <c r="A137" s="0" t="str">
-        <v>6076</v>
+        <v>6083</v>
       </c>
       <c r="B137" s="0" t="str">
-        <v>1004185</v>
+        <v>1004192</v>
       </c>
     </row>
     <row r="138" spans="1:2" customFormat="false">
       <c r="A138" s="0" t="str">
-        <v>6077</v>
+        <v>6084</v>
       </c>
       <c r="B138" s="0" t="str">
-        <v>1004186</v>
+        <v>1004193</v>
       </c>
     </row>
     <row r="139" spans="1:2" customFormat="false">
       <c r="A139" s="0" t="str">
-        <v>6078</v>
+        <v>6085</v>
       </c>
       <c r="B139" s="0" t="str">
-        <v>1004187</v>
+        <v>1004194</v>
       </c>
     </row>
     <row r="140" spans="1:2" customFormat="false">
       <c r="A140" s="0" t="str">
-        <v>6079</v>
+        <v>6086</v>
       </c>
       <c r="B140" s="0" t="str">
-        <v>1004188</v>
+        <v>1004195</v>
       </c>
     </row>
     <row r="141" spans="1:2" customFormat="false">
       <c r="A141" s="0" t="str">
-        <v>6080</v>
+        <v>6087</v>
       </c>
       <c r="B141" s="0" t="str">
-        <v>1004189</v>
+        <v>1004196</v>
       </c>
     </row>
     <row r="142" spans="1:2" customFormat="false">
       <c r="A142" s="0" t="str">
-        <v>6081</v>
+        <v>6088</v>
       </c>
       <c r="B142" s="0" t="str">
-        <v>1004190</v>
+        <v>1004197</v>
       </c>
     </row>
     <row r="143" spans="1:2" customFormat="false">
       <c r="A143" s="0" t="str">
-        <v>6082</v>
+        <v>6089</v>
       </c>
       <c r="B143" s="0" t="str">
-        <v>1004191</v>
+        <v>1004198</v>
       </c>
     </row>
     <row r="144" spans="1:2" customFormat="false">
       <c r="A144" s="0" t="str">
-        <v>6083</v>
+        <v>6090</v>
       </c>
       <c r="B144" s="0" t="str">
-        <v>1004192</v>
+        <v>1004199</v>
       </c>
     </row>
     <row r="145" spans="1:2" customFormat="false">
       <c r="A145" s="0" t="str">
-        <v>6084</v>
+        <v>6091</v>
       </c>
       <c r="B145" s="0" t="str">
-        <v>1004193</v>
+        <v>1004200</v>
       </c>
     </row>
     <row r="146" spans="1:2" customFormat="false">
       <c r="A146" s="0" t="str">
-        <v>6085</v>
+        <v>6092</v>
       </c>
       <c r="B146" s="0" t="str">
-        <v>1004194</v>
+        <v>1004201</v>
       </c>
     </row>
     <row r="147" spans="1:2" customFormat="false">
       <c r="A147" s="0" t="str">
-        <v>6086</v>
+        <v>6093</v>
       </c>
       <c r="B147" s="0" t="str">
-        <v>1004195</v>
+        <v>1004202</v>
       </c>
     </row>
     <row r="148" spans="1:2" customFormat="false">
       <c r="A148" s="0" t="str">
-        <v>6087</v>
+        <v>6094</v>
       </c>
       <c r="B148" s="0" t="str">
-        <v>1004196</v>
+        <v>1004203</v>
       </c>
     </row>
     <row r="149" spans="1:2" customFormat="false">
       <c r="A149" s="0" t="str">
-        <v>6088</v>
+        <v>6095</v>
       </c>
       <c r="B149" s="0" t="str">
-        <v>1004197</v>
+        <v>1004204</v>
       </c>
     </row>
     <row r="150" spans="1:2" customFormat="false">
       <c r="A150" s="0" t="str">
-        <v>6089</v>
+        <v>6096</v>
       </c>
       <c r="B150" s="0" t="str">
-        <v>1004198</v>
+        <v>1004205</v>
       </c>
     </row>
     <row r="151" spans="1:2" customFormat="false">
       <c r="A151" s="0" t="str">
-        <v>6090</v>
+        <v>6097</v>
       </c>
       <c r="B151" s="0" t="str">
-        <v>1004199</v>
+        <v>1004206</v>
       </c>
     </row>
     <row r="152" spans="1:2" customFormat="false">
       <c r="A152" s="0" t="str">
-        <v>6091</v>
+        <v>6098</v>
       </c>
       <c r="B152" s="0" t="str">
-        <v>1004200</v>
+        <v>1004207</v>
       </c>
     </row>
     <row r="153" spans="1:2" customFormat="false">
       <c r="A153" s="0" t="str">
-        <v>6092</v>
+        <v>6099</v>
       </c>
       <c r="B153" s="0" t="str">
-        <v>1004201</v>
+        <v>1004208</v>
       </c>
     </row>
     <row r="154" spans="1:2" customFormat="false">
       <c r="A154" s="0" t="str">
-        <v>6093</v>
+        <v>6100</v>
       </c>
       <c r="B154" s="0" t="str">
-        <v>1004202</v>
+        <v>1004209</v>
       </c>
     </row>
     <row r="155" spans="1:2" customFormat="false">
       <c r="A155" s="0" t="str">
-        <v>6094</v>
+        <v>6101</v>
       </c>
       <c r="B155" s="0" t="str">
-        <v>1004203</v>
+        <v>1004210</v>
       </c>
     </row>
     <row r="156" spans="1:2" customFormat="false">
       <c r="A156" s="0" t="str">
-        <v>6095</v>
+        <v>6102</v>
       </c>
       <c r="B156" s="0" t="str">
-        <v>1004204</v>
+        <v>1004211</v>
       </c>
     </row>
     <row r="157" spans="1:2" customFormat="false">
       <c r="A157" s="0" t="str">
-        <v>6096</v>
+        <v>6103</v>
       </c>
       <c r="B157" s="0" t="str">
-        <v>1004205</v>
+        <v>1004212</v>
       </c>
     </row>
     <row r="158" spans="1:2" customFormat="false">
       <c r="A158" s="0" t="str">
-        <v>6097</v>
+        <v>6104</v>
       </c>
       <c r="B158" s="0" t="str">
-        <v>1004206</v>
+        <v>1004213</v>
       </c>
     </row>
     <row r="159" spans="1:2" customFormat="false">
       <c r="A159" s="0" t="str">
-        <v>6098</v>
+        <v>6105</v>
       </c>
       <c r="B159" s="0" t="str">
-        <v>1004207</v>
+        <v>1004214</v>
       </c>
     </row>
     <row r="160" spans="1:2" customFormat="false">
       <c r="A160" s="0" t="str">
-        <v>6099</v>
+        <v>6106</v>
       </c>
       <c r="B160" s="0" t="str">
-        <v>1004208</v>
+        <v>1004215</v>
       </c>
     </row>
     <row r="161" spans="1:2" customFormat="false">
       <c r="A161" s="0" t="str">
-        <v>6100</v>
+        <v>6107</v>
       </c>
       <c r="B161" s="0" t="str">
-        <v>1004209</v>
+        <v>1004216</v>
       </c>
     </row>
     <row r="162" spans="1:2" customFormat="false">
       <c r="A162" s="0" t="str">
-        <v>6101</v>
+        <v>6108</v>
       </c>
       <c r="B162" s="0" t="str">
-        <v>1004210</v>
+        <v>1004217</v>
       </c>
     </row>
     <row r="163" spans="1:2" customFormat="false">
       <c r="A163" s="0" t="str">
-        <v>6102</v>
+        <v>6109</v>
       </c>
       <c r="B163" s="0" t="str">
-        <v>1004211</v>
+        <v>1004218</v>
       </c>
     </row>
     <row r="164" spans="1:2" customFormat="false">
       <c r="A164" s="0" t="str">
-        <v>6103</v>
+        <v>6110</v>
       </c>
       <c r="B164" s="0" t="str">
-        <v>1004212</v>
+        <v>1004219</v>
       </c>
     </row>
     <row r="165" spans="1:2" customFormat="false">
       <c r="A165" s="0" t="str">
-        <v>6104</v>
+        <v>6111</v>
       </c>
       <c r="B165" s="0" t="str">
-        <v>1004213</v>
+        <v>1004220</v>
       </c>
     </row>
     <row r="166" spans="1:2" customFormat="false">
       <c r="A166" s="0" t="str">
-        <v>6105</v>
+        <v>6113</v>
       </c>
       <c r="B166" s="0" t="str">
-        <v>1004214</v>
+        <v>1004222</v>
       </c>
     </row>
     <row r="167" spans="1:2" customFormat="false">
       <c r="A167" s="0" t="str">
-        <v>6106</v>
+        <v>6114</v>
       </c>
       <c r="B167" s="0" t="str">
-        <v>1004215</v>
+        <v>1004223</v>
       </c>
     </row>
     <row r="168" spans="1:2" customFormat="false">
       <c r="A168" s="0" t="str">
-        <v>6107</v>
+        <v>6115</v>
       </c>
       <c r="B168" s="0" t="str">
-        <v>1004216</v>
+        <v>1004224</v>
       </c>
     </row>
     <row r="169" spans="1:2" customFormat="false">
       <c r="A169" s="0" t="str">
-        <v>6108</v>
+        <v>6116</v>
       </c>
       <c r="B169" s="0" t="str">
-        <v>1004217</v>
+        <v>1004225</v>
       </c>
     </row>
     <row r="170" spans="1:2" customFormat="false">
       <c r="A170" s="0" t="str">
-        <v>6109</v>
+        <v>6117</v>
       </c>
       <c r="B170" s="0" t="str">
-        <v>1004218</v>
+        <v>1004226</v>
       </c>
     </row>
     <row r="171" spans="1:2" customFormat="false">
       <c r="A171" s="0" t="str">
-        <v>6110</v>
+        <v>6118</v>
       </c>
       <c r="B171" s="0" t="str">
-        <v>1004219</v>
+        <v>1004227</v>
       </c>
     </row>
     <row r="172" spans="1:2" customFormat="false">
       <c r="A172" s="0" t="str">
-        <v>6111</v>
+        <v>6119</v>
       </c>
       <c r="B172" s="0" t="str">
-        <v>1004220</v>
+        <v>1004228</v>
       </c>
     </row>
     <row r="173" spans="1:2" customFormat="false">
       <c r="A173" s="0" t="str">
-        <v>6113</v>
+        <v>6120</v>
       </c>
       <c r="B173" s="0" t="str">
-        <v>1004222</v>
+        <v>1004229</v>
       </c>
     </row>
     <row r="174" spans="1:2" customFormat="false">
       <c r="A174" s="0" t="str">
-        <v>6114</v>
+        <v>6121</v>
       </c>
       <c r="B174" s="0" t="str">
-        <v>1004223</v>
+        <v>1004230</v>
       </c>
     </row>
     <row r="175" spans="1:2" customFormat="false">
       <c r="A175" s="0" t="str">
-        <v>6115</v>
+        <v>6122</v>
       </c>
       <c r="B175" s="0" t="str">
-        <v>1004224</v>
+        <v>1004231</v>
       </c>
     </row>
     <row r="176" spans="1:2" customFormat="false">
       <c r="A176" s="0" t="str">
-        <v>6116</v>
+        <v>6123</v>
       </c>
       <c r="B176" s="0" t="str">
-        <v>1004225</v>
+        <v>1004232</v>
       </c>
     </row>
     <row r="177" spans="1:2" customFormat="false">
       <c r="A177" s="0" t="str">
-        <v>6117</v>
+        <v>6124</v>
       </c>
       <c r="B177" s="0" t="str">
-        <v>1004226</v>
+        <v>1004233</v>
       </c>
     </row>
     <row r="178" spans="1:2" customFormat="false">
       <c r="A178" s="0" t="str">
-        <v>6118</v>
+        <v>6125</v>
       </c>
       <c r="B178" s="0" t="str">
-        <v>1004227</v>
+        <v>1004234</v>
       </c>
     </row>
     <row r="179" spans="1:2" customFormat="false">
       <c r="A179" s="0" t="str">
-        <v>6119</v>
+        <v>6126</v>
       </c>
       <c r="B179" s="0" t="str">
-        <v>1004228</v>
+        <v>1004235</v>
       </c>
     </row>
     <row r="180" spans="1:2" customFormat="false">
       <c r="A180" s="0" t="str">
-        <v>6120</v>
+        <v>6127</v>
       </c>
       <c r="B180" s="0" t="str">
-        <v>1004229</v>
+        <v>1004236</v>
       </c>
     </row>
     <row r="181" spans="1:2" customFormat="false">
       <c r="A181" s="0" t="str">
-        <v>6121</v>
+        <v>6128</v>
       </c>
       <c r="B181" s="0" t="str">
-        <v>1004230</v>
+        <v>1004237</v>
       </c>
     </row>
     <row r="182" spans="1:2" customFormat="false">
       <c r="A182" s="0" t="str">
-        <v>6122</v>
+        <v>6129</v>
       </c>
       <c r="B182" s="0" t="str">
-        <v>1004231</v>
+        <v>1004238</v>
       </c>
     </row>
     <row r="183" spans="1:2" customFormat="false">
       <c r="A183" s="0" t="str">
-        <v>6123</v>
+        <v>6130</v>
       </c>
       <c r="B183" s="0" t="str">
-        <v>1004232</v>
+        <v>1004239</v>
       </c>
     </row>
     <row r="184" spans="1:2" customFormat="false">
       <c r="A184" s="0" t="str">
-        <v>6124</v>
+        <v>6131</v>
       </c>
       <c r="B184" s="0" t="str">
-        <v>1004233</v>
+        <v>1004240</v>
       </c>
     </row>
     <row r="185" spans="1:2" customFormat="false">
       <c r="A185" s="0" t="str">
-        <v>6125</v>
+        <v>6132</v>
       </c>
       <c r="B185" s="0" t="str">
-        <v>1004234</v>
+        <v>1004241</v>
       </c>
     </row>
     <row r="186" spans="1:2" customFormat="false">
       <c r="A186" s="0" t="str">
-        <v>6126</v>
+        <v>6133</v>
       </c>
       <c r="B186" s="0" t="str">
-        <v>1004235</v>
+        <v>1004242</v>
       </c>
     </row>
     <row r="187" spans="1:2" customFormat="false">
       <c r="A187" s="0" t="str">
-        <v>6127</v>
+        <v>6134</v>
       </c>
       <c r="B187" s="0" t="str">
-        <v>1004236</v>
+        <v>1004243</v>
       </c>
     </row>
     <row r="188" spans="1:2" customFormat="false">
       <c r="A188" s="0" t="str">
-        <v>6128</v>
+        <v>6135</v>
       </c>
       <c r="B188" s="0" t="str">
-        <v>1004237</v>
+        <v>1004244</v>
       </c>
     </row>
     <row r="189" spans="1:2" customFormat="false">
       <c r="A189" s="0" t="str">
-        <v>6129</v>
+        <v>6136</v>
       </c>
       <c r="B189" s="0" t="str">
-        <v>1004238</v>
+        <v>1004245</v>
       </c>
     </row>
     <row r="190" spans="1:2" customFormat="false">
       <c r="A190" s="0" t="str">
-        <v>6130</v>
+        <v>6137</v>
       </c>
       <c r="B190" s="0" t="str">
-        <v>1004239</v>
+        <v>1004246</v>
       </c>
     </row>
     <row r="191" spans="1:2" customFormat="false">
       <c r="A191" s="0" t="str">
-        <v>6131</v>
+        <v>6138</v>
       </c>
       <c r="B191" s="0" t="str">
-        <v>1004240</v>
+        <v>1004247</v>
       </c>
     </row>
     <row r="192" spans="1:2" customFormat="false">
       <c r="A192" s="0" t="str">
-        <v>6132</v>
+        <v>6139</v>
       </c>
       <c r="B192" s="0" t="str">
-        <v>1004241</v>
+        <v>1004248</v>
       </c>
     </row>
     <row r="193" spans="1:2" customFormat="false">
       <c r="A193" s="0" t="str">
-        <v>6133</v>
+        <v>6140</v>
       </c>
       <c r="B193" s="0" t="str">
-        <v>1004242</v>
+        <v>1004249</v>
       </c>
     </row>
     <row r="194" spans="1:2" customFormat="false">
       <c r="A194" s="0" t="str">
-        <v>6134</v>
+        <v>6141</v>
       </c>
       <c r="B194" s="0" t="str">
-        <v>1004243</v>
+        <v>1004250</v>
       </c>
     </row>
     <row r="195" spans="1:2" customFormat="false">
       <c r="A195" s="0" t="str">
-        <v>6135</v>
+        <v>6142</v>
       </c>
       <c r="B195" s="0" t="str">
-        <v>1004244</v>
+        <v>1004251</v>
       </c>
     </row>
     <row r="196" spans="1:2" customFormat="false">
       <c r="A196" s="0" t="str">
-        <v>6136</v>
+        <v>6143</v>
       </c>
       <c r="B196" s="0" t="str">
-        <v>1004245</v>
+        <v>1004252</v>
       </c>
     </row>
     <row r="197" spans="1:2" customFormat="false">
       <c r="A197" s="0" t="str">
-        <v>6137</v>
+        <v>6144</v>
       </c>
       <c r="B197" s="0" t="str">
-        <v>1004246</v>
+        <v>1004253</v>
       </c>
     </row>
     <row r="198" spans="1:2" customFormat="false">
       <c r="A198" s="0" t="str">
-        <v>6138</v>
+        <v>6145</v>
       </c>
       <c r="B198" s="0" t="str">
-        <v>1004247</v>
+        <v>1004254</v>
       </c>
     </row>
     <row r="199" spans="1:2" customFormat="false">
       <c r="A199" s="0" t="str">
-        <v>6139</v>
+        <v>6146</v>
       </c>
       <c r="B199" s="0" t="str">
-        <v>1004248</v>
+        <v>1004255</v>
       </c>
     </row>
     <row r="200" spans="1:2" customFormat="false">
       <c r="A200" s="0" t="str">
-        <v>6140</v>
+        <v>6147</v>
       </c>
       <c r="B200" s="0" t="str">
-        <v>1004249</v>
+        <v>1004256</v>
       </c>
     </row>
     <row r="201" spans="1:2" customFormat="false">
       <c r="A201" s="0" t="str">
-        <v>6141</v>
+        <v>6148</v>
       </c>
       <c r="B201" s="0" t="str">
-        <v>1004250</v>
+        <v>1004257</v>
       </c>
     </row>
     <row r="202" spans="1:2" customFormat="false">
       <c r="A202" s="0" t="str">
-        <v>6142</v>
+        <v>6149</v>
       </c>
       <c r="B202" s="0" t="str">
-        <v>1004251</v>
+        <v>1004258</v>
       </c>
     </row>
     <row r="203" spans="1:2" customFormat="false">
       <c r="A203" s="0" t="str">
-        <v>6143</v>
+        <v>6150</v>
       </c>
       <c r="B203" s="0" t="str">
-        <v>1004252</v>
+        <v>1004259</v>
       </c>
     </row>
     <row r="204" spans="1:2" customFormat="false">
       <c r="A204" s="0" t="str">
-        <v>6144</v>
+        <v>6151</v>
       </c>
       <c r="B204" s="0" t="str">
-        <v>1004253</v>
+        <v>1004260</v>
       </c>
     </row>
     <row r="205" spans="1:2" customFormat="false">
       <c r="A205" s="0" t="str">
-        <v>6145</v>
+        <v>6152</v>
       </c>
       <c r="B205" s="0" t="str">
-        <v>1004254</v>
+        <v>1004261</v>
       </c>
     </row>
     <row r="206" spans="1:2" customFormat="false">
       <c r="A206" s="0" t="str">
-        <v>6146</v>
+        <v>6153</v>
       </c>
       <c r="B206" s="0" t="str">
-        <v>1004255</v>
+        <v>1004262</v>
       </c>
     </row>
     <row r="207" spans="1:2" customFormat="false">
       <c r="A207" s="0" t="str">
-        <v>6147</v>
+        <v>6154</v>
       </c>
       <c r="B207" s="0" t="str">
-        <v>1004256</v>
+        <v>1004263</v>
       </c>
     </row>
     <row r="208" spans="1:2" customFormat="false">
       <c r="A208" s="0" t="str">
-        <v>6148</v>
+        <v>6155</v>
       </c>
       <c r="B208" s="0" t="str">
-        <v>1004257</v>
+        <v>1004264</v>
       </c>
     </row>
     <row r="209" spans="1:2" customFormat="false">
       <c r="A209" s="0" t="str">
-        <v>6149</v>
+        <v>6156</v>
       </c>
       <c r="B209" s="0" t="str">
-        <v>1004258</v>
+        <v>1004265</v>
       </c>
     </row>
     <row r="210" spans="1:2" customFormat="false">
       <c r="A210" s="0" t="str">
-        <v>6150</v>
+        <v>6157</v>
       </c>
       <c r="B210" s="0" t="str">
-        <v>1004259</v>
+        <v>1004266</v>
       </c>
     </row>
     <row r="211" spans="1:2" customFormat="false">
       <c r="A211" s="0" t="str">
-        <v>6151</v>
+        <v>6158</v>
       </c>
       <c r="B211" s="0" t="str">
-        <v>1004260</v>
+        <v>1004267</v>
       </c>
     </row>
     <row r="212" spans="1:2" customFormat="false">
       <c r="A212" s="0" t="str">
-        <v>6152</v>
+        <v>6159</v>
       </c>
       <c r="B212" s="0" t="str">
-        <v>1004261</v>
+        <v>1004268</v>
       </c>
     </row>
     <row r="213" spans="1:2" customFormat="false">
       <c r="A213" s="0" t="str">
-        <v>6153</v>
+        <v>6160</v>
       </c>
       <c r="B213" s="0" t="str">
-        <v>1004262</v>
+        <v>1004269</v>
       </c>
     </row>
     <row r="214" spans="1:2" customFormat="false">
       <c r="A214" s="0" t="str">
-        <v>6154</v>
+        <v>6161</v>
       </c>
       <c r="B214" s="0" t="str">
-        <v>1004263</v>
+        <v>1004270</v>
       </c>
     </row>
     <row r="215" spans="1:2" customFormat="false">
       <c r="A215" s="0" t="str">
-        <v>6155</v>
+        <v>6162</v>
       </c>
       <c r="B215" s="0" t="str">
-        <v>1004264</v>
+        <v>1004271</v>
       </c>
     </row>
     <row r="216" spans="1:2" customFormat="false">
       <c r="A216" s="0" t="str">
-        <v>6156</v>
+        <v>6163</v>
       </c>
       <c r="B216" s="0" t="str">
-        <v>1004265</v>
+        <v>1004272</v>
       </c>
     </row>
     <row r="217" spans="1:2" customFormat="false">
       <c r="A217" s="0" t="str">
-        <v>6157</v>
+        <v>6164</v>
       </c>
       <c r="B217" s="0" t="str">
-        <v>1004266</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" customFormat="false">
-      <c r="A218" s="0" t="str">
-        <v>6158</v>
-      </c>
-      <c r="B218" s="0" t="str">
-        <v>1004267</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" customFormat="false">
-      <c r="A219" s="0" t="str">
-        <v>6159</v>
-      </c>
-      <c r="B219" s="0" t="str">
-        <v>1004268</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" customFormat="false">
-      <c r="A220" s="0" t="str">
-        <v>6160</v>
-      </c>
-      <c r="B220" s="0" t="str">
-        <v>1004269</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" customFormat="false">
-      <c r="A221" s="0" t="str">
-        <v>6161</v>
-      </c>
-      <c r="B221" s="0" t="str">
-        <v>1004270</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" customFormat="false">
-      <c r="A222" s="0" t="str">
-        <v>6162</v>
-      </c>
-      <c r="B222" s="0" t="str">
-        <v>1004271</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" customFormat="false">
-      <c r="A223" s="0" t="str">
-        <v>6163</v>
-      </c>
-      <c r="B223" s="0" t="str">
-        <v>1004272</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" customFormat="false">
-      <c r="A224" s="0" t="str">
-        <v>6164</v>
-      </c>
-      <c r="B224" s="0" t="str">
         <v>1004273</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Push admin page to heroku
</commit_message>
<xml_diff>
--- a/lib/CVHS Locker Template and Guide.xlsx
+++ b/lib/CVHS Locker Template and Guide.xlsx
@@ -37874,242 +37874,242 @@
     </row>
     <row r="67" spans="1:2" customFormat="false">
       <c r="A67" s="0" t="str">
-        <v>72067</v>
+        <v>72068</v>
       </c>
       <c r="B67" s="0" t="str">
-        <v>1005681</v>
+        <v>1005682</v>
       </c>
     </row>
     <row r="68" spans="1:2" customFormat="false">
       <c r="A68" s="0" t="str">
-        <v>72068</v>
+        <v>72069</v>
       </c>
       <c r="B68" s="0" t="str">
-        <v>1005682</v>
+        <v>1005683</v>
       </c>
     </row>
     <row r="69" spans="1:2" customFormat="false">
       <c r="A69" s="0" t="str">
-        <v>72069</v>
+        <v>72070</v>
       </c>
       <c r="B69" s="0" t="str">
-        <v>1005683</v>
+        <v>1005684</v>
       </c>
     </row>
     <row r="70" spans="1:2" customFormat="false">
       <c r="A70" s="0" t="str">
-        <v>72070</v>
+        <v>72071</v>
       </c>
       <c r="B70" s="0" t="str">
-        <v>1005684</v>
+        <v>1005685</v>
       </c>
     </row>
     <row r="71" spans="1:2" customFormat="false">
       <c r="A71" s="0" t="str">
-        <v>72071</v>
+        <v>72072</v>
       </c>
       <c r="B71" s="0" t="str">
-        <v>1005685</v>
+        <v>1005686</v>
       </c>
     </row>
     <row r="72" spans="1:2" customFormat="false">
       <c r="A72" s="0" t="str">
-        <v>72072</v>
+        <v>72073</v>
       </c>
       <c r="B72" s="0" t="str">
-        <v>1005686</v>
+        <v>1005687</v>
       </c>
     </row>
     <row r="73" spans="1:2" customFormat="false">
       <c r="A73" s="0" t="str">
-        <v>72073</v>
+        <v>72074</v>
       </c>
       <c r="B73" s="0" t="str">
-        <v>1005687</v>
+        <v>1005688</v>
       </c>
     </row>
     <row r="74" spans="1:2" customFormat="false">
       <c r="A74" s="0" t="str">
-        <v>72074</v>
+        <v>72075</v>
       </c>
       <c r="B74" s="0" t="str">
-        <v>1005688</v>
+        <v>1005689</v>
       </c>
     </row>
     <row r="75" spans="1:2" customFormat="false">
       <c r="A75" s="0" t="str">
-        <v>72075</v>
+        <v>72076</v>
       </c>
       <c r="B75" s="0" t="str">
-        <v>1005689</v>
+        <v>1005690</v>
       </c>
     </row>
     <row r="76" spans="1:2" customFormat="false">
       <c r="A76" s="0" t="str">
-        <v>72076</v>
+        <v>72077</v>
       </c>
       <c r="B76" s="0" t="str">
-        <v>1005690</v>
+        <v>1005691</v>
       </c>
     </row>
     <row r="77" spans="1:2" customFormat="false">
       <c r="A77" s="0" t="str">
-        <v>72077</v>
+        <v>72078</v>
       </c>
       <c r="B77" s="0" t="str">
-        <v>1005691</v>
+        <v>1005692</v>
       </c>
     </row>
     <row r="78" spans="1:2" customFormat="false">
       <c r="A78" s="0" t="str">
-        <v>72078</v>
+        <v>72079</v>
       </c>
       <c r="B78" s="0" t="str">
-        <v>1005692</v>
+        <v>1005693</v>
       </c>
     </row>
     <row r="79" spans="1:2" customFormat="false">
       <c r="A79" s="0" t="str">
-        <v>72079</v>
+        <v>72080</v>
       </c>
       <c r="B79" s="0" t="str">
-        <v>1005693</v>
+        <v>1005694</v>
       </c>
     </row>
     <row r="80" spans="1:2" customFormat="false">
       <c r="A80" s="0" t="str">
-        <v>72080</v>
+        <v>72081</v>
       </c>
       <c r="B80" s="0" t="str">
-        <v>1005694</v>
+        <v>1005695</v>
       </c>
     </row>
     <row r="81" spans="1:2" customFormat="false">
       <c r="A81" s="0" t="str">
-        <v>72081</v>
+        <v>72082</v>
       </c>
       <c r="B81" s="0" t="str">
-        <v>1005695</v>
+        <v>1005696</v>
       </c>
     </row>
     <row r="82" spans="1:2" customFormat="false">
       <c r="A82" s="0" t="str">
-        <v>72082</v>
+        <v>72083</v>
       </c>
       <c r="B82" s="0" t="str">
-        <v>1005696</v>
+        <v>1005697</v>
       </c>
     </row>
     <row r="83" spans="1:2" customFormat="false">
       <c r="A83" s="0" t="str">
-        <v>72083</v>
+        <v>72084</v>
       </c>
       <c r="B83" s="0" t="str">
-        <v>1005697</v>
+        <v>1005698</v>
       </c>
     </row>
     <row r="84" spans="1:2" customFormat="false">
       <c r="A84" s="0" t="str">
-        <v>72084</v>
+        <v>72085</v>
       </c>
       <c r="B84" s="0" t="str">
-        <v>1005698</v>
+        <v>1005699</v>
       </c>
     </row>
     <row r="85" spans="1:2" customFormat="false">
       <c r="A85" s="0" t="str">
-        <v>72085</v>
+        <v>72086</v>
       </c>
       <c r="B85" s="0" t="str">
-        <v>1005699</v>
+        <v>1005700</v>
       </c>
     </row>
     <row r="86" spans="1:2" customFormat="false">
       <c r="A86" s="0" t="str">
-        <v>72086</v>
+        <v>72087</v>
       </c>
       <c r="B86" s="0" t="str">
-        <v>1005700</v>
+        <v>1005701</v>
       </c>
     </row>
     <row r="87" spans="1:2" customFormat="false">
       <c r="A87" s="0" t="str">
-        <v>72087</v>
+        <v>72088</v>
       </c>
       <c r="B87" s="0" t="str">
-        <v>1005701</v>
+        <v>1005702</v>
       </c>
     </row>
     <row r="88" spans="1:2" customFormat="false">
       <c r="A88" s="0" t="str">
-        <v>72088</v>
+        <v>72089</v>
       </c>
       <c r="B88" s="0" t="str">
-        <v>1005702</v>
+        <v>1005703</v>
       </c>
     </row>
     <row r="89" spans="1:2" customFormat="false">
       <c r="A89" s="0" t="str">
-        <v>72089</v>
+        <v>72090</v>
       </c>
       <c r="B89" s="0" t="str">
-        <v>1005703</v>
+        <v>1005704</v>
       </c>
     </row>
     <row r="90" spans="1:2" customFormat="false">
       <c r="A90" s="0" t="str">
-        <v>72090</v>
+        <v>72091</v>
       </c>
       <c r="B90" s="0" t="str">
-        <v>1005704</v>
+        <v>1005705</v>
       </c>
     </row>
     <row r="91" spans="1:2" customFormat="false">
       <c r="A91" s="0" t="str">
-        <v>72091</v>
+        <v>72092</v>
       </c>
       <c r="B91" s="0" t="str">
-        <v>1005705</v>
+        <v>1005706</v>
       </c>
     </row>
     <row r="92" spans="1:2" customFormat="false">
       <c r="A92" s="0" t="str">
-        <v>72092</v>
+        <v>72093</v>
       </c>
       <c r="B92" s="0" t="str">
-        <v>1005706</v>
+        <v>1005707</v>
       </c>
     </row>
     <row r="93" spans="1:2" customFormat="false">
       <c r="A93" s="0" t="str">
-        <v>72093</v>
+        <v>72094</v>
       </c>
       <c r="B93" s="0" t="str">
-        <v>1005707</v>
+        <v>1005708</v>
       </c>
     </row>
     <row r="94" spans="1:2" customFormat="false">
       <c r="A94" s="0" t="str">
-        <v>72094</v>
+        <v>72095</v>
       </c>
       <c r="B94" s="0" t="str">
-        <v>1005708</v>
+        <v>1005709</v>
       </c>
     </row>
     <row r="95" spans="1:2" customFormat="false">
       <c r="A95" s="0" t="str">
-        <v>72095</v>
+        <v>72096</v>
       </c>
       <c r="B95" s="0" t="str">
-        <v>1005709</v>
+        <v>1005710</v>
       </c>
     </row>
     <row r="96" spans="1:2" customFormat="false">
       <c r="A96" s="0" t="str">
-        <v>72096</v>
+        <v>72067</v>
       </c>
       <c r="B96" s="0" t="str">
-        <v>1005710</v>
+        <v>1005681</v>
       </c>
     </row>
   </sheetData>

</xml_diff>